<commit_message>
- fixed the excel sheet to include 'project record v1' tab
</commit_message>
<xml_diff>
--- a/tests/UnitTests/Rsp.IrasPortal.UnitTests/Data/ValidQuestionSet.xlsx
+++ b/tests/UnitTests/Rsp.IrasPortal.UnitTests/Data/ValidQuestionSet.xlsx
@@ -5,16 +5,16 @@
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarisAmin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\rsp-iras-portal\tests\UnitTests\Rsp.IrasPortal.UnitTests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756FD34A-0B0E-4370-AD5C-9B1FC34AC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C4BAB-E22A-4557-8BCB-36121EC81D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="16425" firstSheet="2" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="29" r:id="rId1"/>
-    <sheet name="A" sheetId="21" r:id="rId2"/>
+    <sheet name="project record v1" sheetId="21" r:id="rId2"/>
     <sheet name="B" sheetId="24" r:id="rId3"/>
     <sheet name="C1" sheetId="25" r:id="rId4"/>
     <sheet name="C2" sheetId="10" r:id="rId5"/>
@@ -37,9 +37,9 @@
     <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">A!$A$1:$R$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'App1'!$A$14:$P$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">B!$A$1:$R$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'project record v1'!$A$1:$R$3</definedName>
     <definedName name="Conformance" localSheetId="0">'[1]App3 Dropdowns'!$D$2:$D$5</definedName>
     <definedName name="Conformance">'App3 Dropdowns'!$D$2:$D$5</definedName>
     <definedName name="DataType" localSheetId="0">'[1]App3 Dropdowns'!$C$2:$C$12</definedName>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1306">
   <si>
     <t>Master Application Questions</t>
   </si>
@@ -6255,6 +6255,9 @@
   </si>
   <si>
     <t>Short project title (Minimal dataset)</t>
+  </si>
+  <si>
+    <t>project record v1</t>
   </si>
 </sst>
 </file>
@@ -8493,15 +8496,54 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8529,45 +8571,6 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8580,6 +8583,219 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8616,12 +8832,6 @@
     <xf numFmtId="0" fontId="5" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8646,212 +8856,20 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8873,21 +8891,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9192,13 +9195,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="2"/>
         </patternFill>
       </fill>
@@ -9207,6 +9203,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9807,8 +9810,8 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9853,10 +9856,10 @@
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A2" s="318" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="321" t="s">
+      <c r="A2" s="329" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B2" s="334" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="180" t="s">
@@ -9882,8 +9885,8 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="319"/>
-      <c r="B3" s="322"/>
+      <c r="A3" s="333"/>
+      <c r="B3" s="335"/>
       <c r="C3" s="173" t="s">
         <v>14</v>
       </c>
@@ -9907,8 +9910,8 @@
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="320"/>
-      <c r="B4" s="323"/>
+      <c r="A4" s="330"/>
+      <c r="B4" s="336"/>
       <c r="C4" s="190" t="s">
         <v>16</v>
       </c>
@@ -9929,10 +9932,10 @@
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="318" t="s">
+      <c r="A5" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="324" t="s">
+      <c r="B5" s="337" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="180" t="s">
@@ -9951,8 +9954,8 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="319"/>
-      <c r="B6" s="325"/>
+      <c r="A6" s="333"/>
+      <c r="B6" s="338"/>
       <c r="C6" s="173" t="s">
         <v>20</v>
       </c>
@@ -9971,8 +9974,8 @@
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="319"/>
-      <c r="B7" s="325"/>
+      <c r="A7" s="333"/>
+      <c r="B7" s="338"/>
       <c r="C7" s="173" t="s">
         <v>21</v>
       </c>
@@ -9993,8 +9996,8 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="319"/>
-      <c r="B8" s="325"/>
+      <c r="A8" s="333"/>
+      <c r="B8" s="338"/>
       <c r="C8" s="173" t="s">
         <v>23</v>
       </c>
@@ -10007,8 +10010,8 @@
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="319"/>
-      <c r="B9" s="325"/>
+      <c r="A9" s="333"/>
+      <c r="B9" s="338"/>
       <c r="C9" s="173" t="s">
         <v>24</v>
       </c>
@@ -10025,8 +10028,8 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="319"/>
-      <c r="B10" s="325"/>
+      <c r="A10" s="333"/>
+      <c r="B10" s="338"/>
       <c r="C10" s="191" t="s">
         <v>25</v>
       </c>
@@ -10040,8 +10043,8 @@
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="319"/>
-      <c r="B11" s="325"/>
+      <c r="A11" s="333"/>
+      <c r="B11" s="338"/>
       <c r="C11" s="191" t="s">
         <v>26</v>
       </c>
@@ -10061,8 +10064,8 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="319"/>
-      <c r="B12" s="325"/>
+      <c r="A12" s="333"/>
+      <c r="B12" s="338"/>
       <c r="C12" s="191" t="s">
         <v>27</v>
       </c>
@@ -10082,8 +10085,8 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="57" x14ac:dyDescent="0.25">
-      <c r="A13" s="319"/>
-      <c r="B13" s="325"/>
+      <c r="A13" s="333"/>
+      <c r="B13" s="338"/>
       <c r="C13" s="191" t="s">
         <v>28</v>
       </c>
@@ -10108,8 +10111,8 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="319"/>
-      <c r="B14" s="325"/>
+      <c r="A14" s="333"/>
+      <c r="B14" s="338"/>
       <c r="C14" s="191" t="s">
         <v>29</v>
       </c>
@@ -10127,8 +10130,8 @@
       <c r="Q14" s="90"/>
     </row>
     <row r="15" spans="1:17" s="79" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="319"/>
-      <c r="B15" s="325"/>
+      <c r="A15" s="333"/>
+      <c r="B15" s="338"/>
       <c r="C15" s="191" t="s">
         <v>30</v>
       </c>
@@ -10154,8 +10157,8 @@
       <c r="Q15" s="90"/>
     </row>
     <row r="16" spans="1:17" s="79" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="320"/>
-      <c r="B16" s="326"/>
+      <c r="A16" s="330"/>
+      <c r="B16" s="339"/>
       <c r="C16" s="193" t="s">
         <v>32</v>
       </c>
@@ -10248,16 +10251,16 @@
       <c r="Q19" s="90"/>
     </row>
     <row r="20" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="327" t="s">
+      <c r="A20" s="340" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="321" t="s">
+      <c r="B20" s="334" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="335" t="s">
+      <c r="D20" s="323" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="238"/>
@@ -10271,12 +10274,12 @@
       <c r="Q20" s="90"/>
     </row>
     <row r="21" spans="1:17" s="79" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="328"/>
-      <c r="B21" s="322"/>
+      <c r="A21" s="341"/>
+      <c r="B21" s="335"/>
       <c r="C21" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="336"/>
+      <c r="D21" s="324"/>
       <c r="F21" s="238"/>
       <c r="G21" s="238"/>
       <c r="H21" s="238"/>
@@ -10288,8 +10291,8 @@
       <c r="Q21" s="90"/>
     </row>
     <row r="22" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="329"/>
-      <c r="B22" s="323"/>
+      <c r="A22" s="342"/>
+      <c r="B22" s="336"/>
       <c r="C22" s="169" t="s">
         <v>49</v>
       </c>
@@ -10320,16 +10323,16 @@
       <c r="Q23" s="90"/>
     </row>
     <row r="24" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="337" t="s">
+      <c r="A24" s="325" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="338" t="s">
+      <c r="B24" s="326" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="335" t="s">
+      <c r="D24" s="323" t="s">
         <v>57</v>
       </c>
       <c r="F24"/>
@@ -10343,12 +10346,12 @@
       <c r="Q24" s="132"/>
     </row>
     <row r="25" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="331"/>
-      <c r="B25" s="339"/>
+      <c r="A25" s="319"/>
+      <c r="B25" s="327"/>
       <c r="C25" s="172" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="340"/>
+      <c r="D25" s="328"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
@@ -10360,10 +10363,10 @@
       <c r="Q25" s="132"/>
     </row>
     <row r="26" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="318" t="s">
+      <c r="A26" s="329" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="341" t="s">
+      <c r="B26" s="331" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="192" t="s">
@@ -10383,8 +10386,8 @@
       <c r="Q26" s="132"/>
     </row>
     <row r="27" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="320"/>
-      <c r="B27" s="342"/>
+      <c r="A27" s="330"/>
+      <c r="B27" s="332"/>
       <c r="C27" s="190" t="s">
         <v>63</v>
       </c>
@@ -10442,10 +10445,10 @@
       <c r="Q29" s="132"/>
     </row>
     <row r="30" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="330" t="s">
+      <c r="A30" s="318" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="333" t="s">
+      <c r="B30" s="321" t="s">
         <v>72</v>
       </c>
       <c r="C30" s="174" t="s">
@@ -10465,8 +10468,8 @@
       <c r="Q30" s="132"/>
     </row>
     <row r="31" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="331"/>
-      <c r="B31" s="333"/>
+      <c r="A31" s="319"/>
+      <c r="B31" s="321"/>
       <c r="C31" s="191" t="s">
         <v>75</v>
       </c>
@@ -10484,8 +10487,8 @@
       <c r="Q31" s="132"/>
     </row>
     <row r="32" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="331"/>
-      <c r="B32" s="333"/>
+      <c r="A32" s="319"/>
+      <c r="B32" s="321"/>
       <c r="C32" s="191" t="s">
         <v>77</v>
       </c>
@@ -10503,8 +10506,8 @@
       <c r="Q32" s="132"/>
     </row>
     <row r="33" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="332"/>
-      <c r="B33" s="334"/>
+      <c r="A33" s="320"/>
+      <c r="B33" s="322"/>
       <c r="C33" s="175"/>
       <c r="D33" s="161"/>
       <c r="F33" s="92"/>
@@ -10733,6 +10736,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="D20:D21"/>
@@ -10741,12 +10750,6 @@
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A16"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" location="A!E5" display="Project details" xr:uid="{4428746E-4300-4BD2-985A-60358BBE6AB0}"/>
@@ -13687,10 +13690,10 @@
       <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="376" t="s">
+      <c r="B4" s="404" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="377"/>
+      <c r="C4" s="405"/>
       <c r="D4" s="63" t="s">
         <v>242</v>
       </c>
@@ -13733,8 +13736,8 @@
       <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="1:17" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="378"/>
-      <c r="C5" s="379"/>
+      <c r="B5" s="406"/>
+      <c r="C5" s="407"/>
       <c r="D5" s="64" t="s">
         <v>243</v>
       </c>
@@ -13779,7 +13782,7 @@
       <c r="B6" s="207">
         <v>1</v>
       </c>
-      <c r="C6" s="383" t="s">
+      <c r="C6" s="411" t="s">
         <v>255</v>
       </c>
       <c r="D6" s="43" t="s">
@@ -13826,7 +13829,7 @@
       <c r="B7" s="42">
         <v>2</v>
       </c>
-      <c r="C7" s="383"/>
+      <c r="C7" s="411"/>
       <c r="D7" s="46" t="s">
         <v>258</v>
       </c>
@@ -13871,7 +13874,7 @@
       <c r="B8" s="42">
         <v>3</v>
       </c>
-      <c r="C8" s="383"/>
+      <c r="C8" s="411"/>
       <c r="D8" s="46" t="s">
         <v>259</v>
       </c>
@@ -13904,7 +13907,7 @@
       <c r="B9" s="42">
         <v>4</v>
       </c>
-      <c r="C9" s="383"/>
+      <c r="C9" s="411"/>
       <c r="D9" s="46" t="s">
         <v>260</v>
       </c>
@@ -13932,7 +13935,7 @@
       <c r="B10" s="199">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C10" s="383"/>
+      <c r="C10" s="411"/>
       <c r="D10" s="198" t="s">
         <v>261</v>
       </c>
@@ -13975,7 +13978,7 @@
       <c r="B11" s="42">
         <v>5</v>
       </c>
-      <c r="C11" s="383"/>
+      <c r="C11" s="411"/>
       <c r="D11" s="46" t="s">
         <v>262</v>
       </c>
@@ -14018,7 +14021,7 @@
       <c r="B12" s="42">
         <v>6</v>
       </c>
-      <c r="C12" s="383"/>
+      <c r="C12" s="411"/>
       <c r="D12" s="46" t="s">
         <v>263</v>
       </c>
@@ -14060,7 +14063,7 @@
       <c r="B13" s="42">
         <v>7</v>
       </c>
-      <c r="C13" s="384"/>
+      <c r="C13" s="412"/>
       <c r="D13" s="48" t="s">
         <v>264</v>
       </c>
@@ -14101,24 +14104,24 @@
     </row>
     <row r="15" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
-      <c r="C15" s="373" t="s">
+      <c r="C15" s="401" t="s">
         <v>265</v>
       </c>
-      <c r="D15" s="374"/>
-      <c r="E15" s="385" t="s">
+      <c r="D15" s="402"/>
+      <c r="E15" s="413" t="s">
         <v>266</v>
       </c>
-      <c r="F15" s="386"/>
-      <c r="G15" s="386"/>
-      <c r="H15" s="386"/>
-      <c r="I15" s="386"/>
-      <c r="J15" s="386"/>
-      <c r="K15" s="386"/>
-      <c r="L15" s="386"/>
-      <c r="M15" s="386"/>
-      <c r="N15" s="386"/>
-      <c r="O15" s="386"/>
-      <c r="P15" s="386"/>
+      <c r="F15" s="414"/>
+      <c r="G15" s="414"/>
+      <c r="H15" s="414"/>
+      <c r="I15" s="414"/>
+      <c r="J15" s="414"/>
+      <c r="K15" s="414"/>
+      <c r="L15" s="414"/>
+      <c r="M15" s="414"/>
+      <c r="N15" s="414"/>
+      <c r="O15" s="414"/>
+      <c r="P15" s="414"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
@@ -14127,37 +14130,37 @@
       <c r="D16" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="381" t="s">
+      <c r="E16" s="409" t="s">
         <v>268</v>
       </c>
-      <c r="F16" s="381"/>
-      <c r="G16" s="381"/>
-      <c r="H16" s="381"/>
-      <c r="I16" s="381"/>
-      <c r="J16" s="381"/>
-      <c r="K16" s="381"/>
-      <c r="L16" s="381"/>
-      <c r="M16" s="381"/>
-      <c r="N16" s="381"/>
-      <c r="O16" s="381"/>
-      <c r="P16" s="381"/>
+      <c r="F16" s="409"/>
+      <c r="G16" s="409"/>
+      <c r="H16" s="409"/>
+      <c r="I16" s="409"/>
+      <c r="J16" s="409"/>
+      <c r="K16" s="409"/>
+      <c r="L16" s="409"/>
+      <c r="M16" s="409"/>
+      <c r="N16" s="409"/>
+      <c r="O16" s="409"/>
+      <c r="P16" s="409"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="375" t="s">
+      <c r="D17" s="403" t="s">
         <v>269</v>
       </c>
-      <c r="E17" s="375"/>
-      <c r="F17" s="375"/>
-      <c r="G17" s="375"/>
-      <c r="H17" s="375"/>
-      <c r="I17" s="375"/>
-      <c r="J17" s="375"/>
-      <c r="K17" s="375"/>
-      <c r="L17" s="375"/>
-      <c r="M17" s="375"/>
-      <c r="N17" s="375"/>
-      <c r="O17" s="375"/>
-      <c r="P17" s="375"/>
+      <c r="E17" s="403"/>
+      <c r="F17" s="403"/>
+      <c r="G17" s="403"/>
+      <c r="H17" s="403"/>
+      <c r="I17" s="403"/>
+      <c r="J17" s="403"/>
+      <c r="K17" s="403"/>
+      <c r="L17" s="403"/>
+      <c r="M17" s="403"/>
+      <c r="N17" s="403"/>
+      <c r="O17" s="403"/>
+      <c r="P17" s="403"/>
     </row>
     <row r="18" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="42">
@@ -14166,20 +14169,20 @@
       <c r="D18" s="68" t="s">
         <v>270</v>
       </c>
-      <c r="E18" s="380" t="s">
+      <c r="E18" s="408" t="s">
         <v>271</v>
       </c>
-      <c r="F18" s="381"/>
-      <c r="G18" s="381"/>
-      <c r="H18" s="381"/>
-      <c r="I18" s="381"/>
-      <c r="J18" s="381"/>
-      <c r="K18" s="381"/>
-      <c r="L18" s="381"/>
-      <c r="M18" s="381"/>
-      <c r="N18" s="381"/>
-      <c r="O18" s="381"/>
-      <c r="P18" s="381"/>
+      <c r="F18" s="409"/>
+      <c r="G18" s="409"/>
+      <c r="H18" s="409"/>
+      <c r="I18" s="409"/>
+      <c r="J18" s="409"/>
+      <c r="K18" s="409"/>
+      <c r="L18" s="409"/>
+      <c r="M18" s="409"/>
+      <c r="N18" s="409"/>
+      <c r="O18" s="409"/>
+      <c r="P18" s="409"/>
     </row>
     <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="42">
@@ -14188,20 +14191,20 @@
       <c r="D19" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="E19" s="371" t="s">
+      <c r="E19" s="399" t="s">
         <v>273</v>
       </c>
-      <c r="F19" s="372"/>
-      <c r="G19" s="372"/>
-      <c r="H19" s="372"/>
-      <c r="I19" s="372"/>
-      <c r="J19" s="372"/>
-      <c r="K19" s="372"/>
-      <c r="L19" s="372"/>
-      <c r="M19" s="372"/>
-      <c r="N19" s="372"/>
-      <c r="O19" s="372"/>
-      <c r="P19" s="372"/>
+      <c r="F19" s="400"/>
+      <c r="G19" s="400"/>
+      <c r="H19" s="400"/>
+      <c r="I19" s="400"/>
+      <c r="J19" s="400"/>
+      <c r="K19" s="400"/>
+      <c r="L19" s="400"/>
+      <c r="M19" s="400"/>
+      <c r="N19" s="400"/>
+      <c r="O19" s="400"/>
+      <c r="P19" s="400"/>
     </row>
     <row r="20" spans="1:16" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="42">
@@ -14210,20 +14213,20 @@
       <c r="D20" s="53" t="s">
         <v>274</v>
       </c>
-      <c r="E20" s="371" t="s">
+      <c r="E20" s="399" t="s">
         <v>275</v>
       </c>
-      <c r="F20" s="372"/>
-      <c r="G20" s="372"/>
-      <c r="H20" s="372"/>
-      <c r="I20" s="372"/>
-      <c r="J20" s="372"/>
-      <c r="K20" s="372"/>
-      <c r="L20" s="372"/>
-      <c r="M20" s="372"/>
-      <c r="N20" s="372"/>
-      <c r="O20" s="372"/>
-      <c r="P20" s="372"/>
+      <c r="F20" s="400"/>
+      <c r="G20" s="400"/>
+      <c r="H20" s="400"/>
+      <c r="I20" s="400"/>
+      <c r="J20" s="400"/>
+      <c r="K20" s="400"/>
+      <c r="L20" s="400"/>
+      <c r="M20" s="400"/>
+      <c r="N20" s="400"/>
+      <c r="O20" s="400"/>
+      <c r="P20" s="400"/>
     </row>
     <row r="21" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="42">
@@ -14232,20 +14235,20 @@
       <c r="D21" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="E21" s="382" t="s">
+      <c r="E21" s="410" t="s">
         <v>277</v>
       </c>
-      <c r="F21" s="382"/>
-      <c r="G21" s="382"/>
-      <c r="H21" s="382"/>
-      <c r="I21" s="382"/>
-      <c r="J21" s="382"/>
-      <c r="K21" s="382"/>
-      <c r="L21" s="382"/>
-      <c r="M21" s="382"/>
-      <c r="N21" s="382"/>
-      <c r="O21" s="382"/>
-      <c r="P21" s="382"/>
+      <c r="F21" s="410"/>
+      <c r="G21" s="410"/>
+      <c r="H21" s="410"/>
+      <c r="I21" s="410"/>
+      <c r="J21" s="410"/>
+      <c r="K21" s="410"/>
+      <c r="L21" s="410"/>
+      <c r="M21" s="410"/>
+      <c r="N21" s="410"/>
+      <c r="O21" s="410"/>
+      <c r="P21" s="410"/>
     </row>
     <row r="22" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="199">
@@ -14254,20 +14257,20 @@
       <c r="D22" s="208" t="s">
         <v>278</v>
       </c>
-      <c r="E22" s="387" t="s">
+      <c r="E22" s="415" t="s">
         <v>279</v>
       </c>
-      <c r="F22" s="388"/>
-      <c r="G22" s="388"/>
-      <c r="H22" s="388"/>
-      <c r="I22" s="388"/>
-      <c r="J22" s="388"/>
-      <c r="K22" s="388"/>
-      <c r="L22" s="388"/>
-      <c r="M22" s="388"/>
-      <c r="N22" s="388"/>
-      <c r="O22" s="388"/>
-      <c r="P22" s="389"/>
+      <c r="F22" s="416"/>
+      <c r="G22" s="416"/>
+      <c r="H22" s="416"/>
+      <c r="I22" s="416"/>
+      <c r="J22" s="416"/>
+      <c r="K22" s="416"/>
+      <c r="L22" s="416"/>
+      <c r="M22" s="416"/>
+      <c r="N22" s="416"/>
+      <c r="O22" s="416"/>
+      <c r="P22" s="417"/>
     </row>
     <row r="23" spans="1:16" ht="152.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="42">
@@ -14276,20 +14279,20 @@
       <c r="D23" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="E23" s="371" t="s">
+      <c r="E23" s="399" t="s">
         <v>281</v>
       </c>
-      <c r="F23" s="372"/>
-      <c r="G23" s="372"/>
-      <c r="H23" s="372"/>
-      <c r="I23" s="372"/>
-      <c r="J23" s="372"/>
-      <c r="K23" s="372"/>
-      <c r="L23" s="372"/>
-      <c r="M23" s="372"/>
-      <c r="N23" s="372"/>
-      <c r="O23" s="372"/>
-      <c r="P23" s="372"/>
+      <c r="F23" s="400"/>
+      <c r="G23" s="400"/>
+      <c r="H23" s="400"/>
+      <c r="I23" s="400"/>
+      <c r="J23" s="400"/>
+      <c r="K23" s="400"/>
+      <c r="L23" s="400"/>
+      <c r="M23" s="400"/>
+      <c r="N23" s="400"/>
+      <c r="O23" s="400"/>
+      <c r="P23" s="400"/>
     </row>
     <row r="24" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="42">
@@ -14298,20 +14301,20 @@
       <c r="D24" s="53" t="s">
         <v>282</v>
       </c>
-      <c r="E24" s="371" t="s">
+      <c r="E24" s="399" t="s">
         <v>283</v>
       </c>
-      <c r="F24" s="372"/>
-      <c r="G24" s="372"/>
-      <c r="H24" s="372"/>
-      <c r="I24" s="372"/>
-      <c r="J24" s="372"/>
-      <c r="K24" s="372"/>
-      <c r="L24" s="372"/>
-      <c r="M24" s="372"/>
-      <c r="N24" s="372"/>
-      <c r="O24" s="372"/>
-      <c r="P24" s="372"/>
+      <c r="F24" s="400"/>
+      <c r="G24" s="400"/>
+      <c r="H24" s="400"/>
+      <c r="I24" s="400"/>
+      <c r="J24" s="400"/>
+      <c r="K24" s="400"/>
+      <c r="L24" s="400"/>
+      <c r="M24" s="400"/>
+      <c r="N24" s="400"/>
+      <c r="O24" s="400"/>
+      <c r="P24" s="400"/>
     </row>
     <row r="25" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="42">
@@ -14320,20 +14323,20 @@
       <c r="D25" s="53" t="s">
         <v>284</v>
       </c>
-      <c r="E25" s="371" t="s">
+      <c r="E25" s="399" t="s">
         <v>285</v>
       </c>
-      <c r="F25" s="372"/>
-      <c r="G25" s="372"/>
-      <c r="H25" s="372"/>
-      <c r="I25" s="372"/>
-      <c r="J25" s="372"/>
-      <c r="K25" s="372"/>
-      <c r="L25" s="372"/>
-      <c r="M25" s="372"/>
-      <c r="N25" s="372"/>
-      <c r="O25" s="372"/>
-      <c r="P25" s="372"/>
+      <c r="F25" s="400"/>
+      <c r="G25" s="400"/>
+      <c r="H25" s="400"/>
+      <c r="I25" s="400"/>
+      <c r="J25" s="400"/>
+      <c r="K25" s="400"/>
+      <c r="L25" s="400"/>
+      <c r="M25" s="400"/>
+      <c r="N25" s="400"/>
+      <c r="O25" s="400"/>
+      <c r="P25" s="400"/>
     </row>
     <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="78" t="s">
@@ -14349,184 +14352,184 @@
       <c r="E30" s="81"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="390" t="s">
+      <c r="B31" s="398" t="s">
         <v>287</v>
       </c>
-      <c r="C31" s="390"/>
+      <c r="C31" s="398"/>
       <c r="D31" s="82" t="s">
         <v>288</v>
       </c>
-      <c r="E31" s="390" t="s">
+      <c r="E31" s="398" t="s">
         <v>289</v>
       </c>
-      <c r="F31" s="390"/>
-      <c r="G31" s="390"/>
-      <c r="H31" s="390"/>
-      <c r="I31" s="390"/>
-      <c r="J31" s="390"/>
-      <c r="K31" s="390"/>
+      <c r="F31" s="398"/>
+      <c r="G31" s="398"/>
+      <c r="H31" s="398"/>
+      <c r="I31" s="398"/>
+      <c r="J31" s="398"/>
+      <c r="K31" s="398"/>
     </row>
     <row r="32" spans="1:16" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="392" t="s">
+      <c r="B32" s="388" t="s">
         <v>290</v>
       </c>
-      <c r="C32" s="392"/>
+      <c r="C32" s="388"/>
       <c r="D32" s="84" t="s">
         <v>291</v>
       </c>
-      <c r="E32" s="391" t="s">
+      <c r="E32" s="389" t="s">
         <v>292</v>
       </c>
-      <c r="F32" s="391"/>
-      <c r="G32" s="391"/>
-      <c r="H32" s="391"/>
-      <c r="I32" s="391"/>
-      <c r="J32" s="391"/>
-      <c r="K32" s="391"/>
+      <c r="F32" s="389"/>
+      <c r="G32" s="389"/>
+      <c r="H32" s="389"/>
+      <c r="I32" s="389"/>
+      <c r="J32" s="389"/>
+      <c r="K32" s="389"/>
     </row>
     <row r="33" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="392" t="s">
+      <c r="B33" s="388" t="s">
         <v>293</v>
       </c>
-      <c r="C33" s="392"/>
+      <c r="C33" s="388"/>
       <c r="D33" s="85" t="s">
         <v>294</v>
       </c>
-      <c r="E33" s="391" t="s">
+      <c r="E33" s="389" t="s">
         <v>295</v>
       </c>
-      <c r="F33" s="391"/>
-      <c r="G33" s="391"/>
-      <c r="H33" s="391"/>
-      <c r="I33" s="391"/>
-      <c r="J33" s="391"/>
-      <c r="K33" s="391"/>
+      <c r="F33" s="389"/>
+      <c r="G33" s="389"/>
+      <c r="H33" s="389"/>
+      <c r="I33" s="389"/>
+      <c r="J33" s="389"/>
+      <c r="K33" s="389"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="392" t="s">
+      <c r="B34" s="388" t="s">
         <v>296</v>
       </c>
-      <c r="C34" s="392"/>
+      <c r="C34" s="388"/>
       <c r="D34" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="E34" s="393" t="s">
+      <c r="E34" s="391" t="s">
         <v>298</v>
       </c>
-      <c r="F34" s="393"/>
-      <c r="G34" s="393"/>
-      <c r="H34" s="393"/>
-      <c r="I34" s="393"/>
-      <c r="J34" s="393"/>
-      <c r="K34" s="393"/>
+      <c r="F34" s="391"/>
+      <c r="G34" s="391"/>
+      <c r="H34" s="391"/>
+      <c r="I34" s="391"/>
+      <c r="J34" s="391"/>
+      <c r="K34" s="391"/>
     </row>
     <row r="35" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="394" t="s">
+      <c r="B35" s="390" t="s">
         <v>299</v>
       </c>
-      <c r="C35" s="394"/>
+      <c r="C35" s="390"/>
       <c r="D35" s="86" t="s">
         <v>300</v>
       </c>
-      <c r="E35" s="391" t="s">
+      <c r="E35" s="389" t="s">
         <v>301</v>
       </c>
-      <c r="F35" s="391"/>
-      <c r="G35" s="391"/>
-      <c r="H35" s="391"/>
-      <c r="I35" s="391"/>
-      <c r="J35" s="391"/>
-      <c r="K35" s="391"/>
+      <c r="F35" s="389"/>
+      <c r="G35" s="389"/>
+      <c r="H35" s="389"/>
+      <c r="I35" s="389"/>
+      <c r="J35" s="389"/>
+      <c r="K35" s="389"/>
     </row>
     <row r="36" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="392" t="s">
+      <c r="B36" s="388" t="s">
         <v>302</v>
       </c>
-      <c r="C36" s="392"/>
+      <c r="C36" s="388"/>
       <c r="D36" s="83" t="s">
         <v>303</v>
       </c>
-      <c r="E36" s="393" t="s">
+      <c r="E36" s="391" t="s">
         <v>304</v>
       </c>
-      <c r="F36" s="395"/>
-      <c r="G36" s="395"/>
-      <c r="H36" s="395"/>
-      <c r="I36" s="395"/>
-      <c r="J36" s="395"/>
-      <c r="K36" s="395"/>
+      <c r="F36" s="397"/>
+      <c r="G36" s="397"/>
+      <c r="H36" s="397"/>
+      <c r="I36" s="397"/>
+      <c r="J36" s="397"/>
+      <c r="K36" s="397"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="392" t="s">
+      <c r="B37" s="388" t="s">
         <v>305</v>
       </c>
-      <c r="C37" s="392"/>
+      <c r="C37" s="388"/>
       <c r="D37" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="E37" s="391" t="s">
+      <c r="E37" s="389" t="s">
         <v>307</v>
       </c>
-      <c r="F37" s="391"/>
-      <c r="G37" s="391"/>
-      <c r="H37" s="391"/>
-      <c r="I37" s="391"/>
-      <c r="J37" s="391"/>
-      <c r="K37" s="391"/>
+      <c r="F37" s="389"/>
+      <c r="G37" s="389"/>
+      <c r="H37" s="389"/>
+      <c r="I37" s="389"/>
+      <c r="J37" s="389"/>
+      <c r="K37" s="389"/>
     </row>
     <row r="38" spans="1:11" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="396" t="s">
+      <c r="B38" s="392" t="s">
         <v>308</v>
       </c>
-      <c r="C38" s="397"/>
+      <c r="C38" s="393"/>
       <c r="D38" s="86" t="s">
         <v>309</v>
       </c>
-      <c r="E38" s="398" t="s">
+      <c r="E38" s="394" t="s">
         <v>310</v>
       </c>
-      <c r="F38" s="399"/>
-      <c r="G38" s="399"/>
-      <c r="H38" s="399"/>
-      <c r="I38" s="399"/>
-      <c r="J38" s="399"/>
-      <c r="K38" s="400"/>
+      <c r="F38" s="395"/>
+      <c r="G38" s="395"/>
+      <c r="H38" s="395"/>
+      <c r="I38" s="395"/>
+      <c r="J38" s="395"/>
+      <c r="K38" s="396"/>
     </row>
     <row r="39" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="394" t="s">
+      <c r="B39" s="390" t="s">
         <v>311</v>
       </c>
-      <c r="C39" s="394"/>
+      <c r="C39" s="390"/>
       <c r="D39" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="E39" s="393" t="s">
+      <c r="E39" s="391" t="s">
         <v>313</v>
       </c>
-      <c r="F39" s="393"/>
-      <c r="G39" s="393"/>
-      <c r="H39" s="393"/>
-      <c r="I39" s="393"/>
-      <c r="J39" s="393"/>
-      <c r="K39" s="393"/>
+      <c r="F39" s="391"/>
+      <c r="G39" s="391"/>
+      <c r="H39" s="391"/>
+      <c r="I39" s="391"/>
+      <c r="J39" s="391"/>
+      <c r="K39" s="391"/>
     </row>
     <row r="40" spans="1:11" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="392" t="s">
+      <c r="B40" s="388" t="s">
         <v>314</v>
       </c>
-      <c r="C40" s="392"/>
+      <c r="C40" s="388"/>
       <c r="D40" s="84" t="s">
         <v>315</v>
       </c>
-      <c r="E40" s="393" t="s">
+      <c r="E40" s="391" t="s">
         <v>316</v>
       </c>
-      <c r="F40" s="393"/>
-      <c r="G40" s="393"/>
-      <c r="H40" s="393"/>
-      <c r="I40" s="393"/>
-      <c r="J40" s="393"/>
-      <c r="K40" s="393"/>
+      <c r="F40" s="391"/>
+      <c r="G40" s="391"/>
+      <c r="H40" s="391"/>
+      <c r="I40" s="391"/>
+      <c r="J40" s="391"/>
+      <c r="K40" s="391"/>
     </row>
     <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -14544,11 +14547,11 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A47" s="414" t="s">
+      <c r="A47" s="380" t="s">
         <v>319</v>
       </c>
-      <c r="B47" s="412"/>
-      <c r="C47" s="412"/>
+      <c r="B47" s="378"/>
+      <c r="C47" s="378"/>
       <c r="D47" s="141" t="s">
         <v>320</v>
       </c>
@@ -14564,18 +14567,18 @@
       <c r="H47" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="I47" s="411" t="s">
+      <c r="I47" s="377" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="412"/>
-      <c r="K47" s="413"/>
+      <c r="J47" s="378"/>
+      <c r="K47" s="379"/>
     </row>
     <row r="48" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="403" t="s">
+      <c r="A48" s="373" t="s">
         <v>323</v>
       </c>
-      <c r="B48" s="404"/>
-      <c r="C48" s="404"/>
+      <c r="B48" s="366"/>
+      <c r="C48" s="366"/>
       <c r="D48" s="91" t="s">
         <v>324</v>
       </c>
@@ -14591,37 +14594,37 @@
       <c r="H48" s="87" t="s">
         <v>326</v>
       </c>
-      <c r="I48" s="415" t="s">
+      <c r="I48" s="381" t="s">
         <v>327</v>
       </c>
-      <c r="J48" s="415"/>
-      <c r="K48" s="416"/>
+      <c r="J48" s="381"/>
+      <c r="K48" s="382"/>
     </row>
     <row r="49" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="403" t="s">
+      <c r="A49" s="373" t="s">
         <v>328</v>
       </c>
-      <c r="B49" s="404"/>
-      <c r="C49" s="404"/>
+      <c r="B49" s="366"/>
+      <c r="C49" s="366"/>
       <c r="D49" s="91" t="s">
         <v>329</v>
       </c>
-      <c r="E49" s="357" t="s">
+      <c r="E49" s="428" t="s">
         <v>330</v>
       </c>
-      <c r="F49" s="357"/>
-      <c r="G49" s="357"/>
-      <c r="H49" s="357"/>
-      <c r="I49" s="357"/>
-      <c r="J49" s="357"/>
-      <c r="K49" s="358"/>
+      <c r="F49" s="428"/>
+      <c r="G49" s="428"/>
+      <c r="H49" s="428"/>
+      <c r="I49" s="428"/>
+      <c r="J49" s="428"/>
+      <c r="K49" s="429"/>
     </row>
     <row r="50" spans="1:11" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="403" t="s">
+      <c r="A50" s="373" t="s">
         <v>331</v>
       </c>
-      <c r="B50" s="404"/>
-      <c r="C50" s="404"/>
+      <c r="B50" s="366"/>
+      <c r="C50" s="366"/>
       <c r="D50" s="126" t="s">
         <v>332</v>
       </c>
@@ -14637,16 +14640,16 @@
       <c r="H50" s="98" t="s">
         <v>334</v>
       </c>
-      <c r="I50" s="415" t="s">
+      <c r="I50" s="381" t="s">
         <v>335</v>
       </c>
-      <c r="J50" s="415"/>
-      <c r="K50" s="416"/>
+      <c r="J50" s="381"/>
+      <c r="K50" s="382"/>
     </row>
     <row r="51" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="403"/>
-      <c r="B51" s="404"/>
-      <c r="C51" s="404"/>
+      <c r="A51" s="373"/>
+      <c r="B51" s="366"/>
+      <c r="C51" s="366"/>
       <c r="D51" s="127" t="s">
         <v>336</v>
       </c>
@@ -14662,19 +14665,19 @@
       <c r="H51" s="87" t="s">
         <v>338</v>
       </c>
-      <c r="I51" s="417" t="s">
+      <c r="I51" s="383" t="s">
         <v>339</v>
       </c>
-      <c r="J51" s="417"/>
-      <c r="K51" s="418"/>
+      <c r="J51" s="383"/>
+      <c r="K51" s="384"/>
     </row>
     <row r="52" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="403" t="s">
+      <c r="A52" s="373" t="s">
         <v>340</v>
       </c>
-      <c r="B52" s="404"/>
-      <c r="C52" s="404"/>
-      <c r="D52" s="410" t="s">
+      <c r="B52" s="366"/>
+      <c r="C52" s="366"/>
+      <c r="D52" s="376" t="s">
         <v>341</v>
       </c>
       <c r="E52" s="137" t="s">
@@ -14689,17 +14692,17 @@
       <c r="H52" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I52" s="419" t="s">
+      <c r="I52" s="368" t="s">
         <v>343</v>
       </c>
-      <c r="J52" s="419"/>
-      <c r="K52" s="420"/>
+      <c r="J52" s="368"/>
+      <c r="K52" s="369"/>
     </row>
     <row r="53" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="405"/>
-      <c r="B53" s="406"/>
-      <c r="C53" s="406"/>
-      <c r="D53" s="410"/>
+      <c r="A53" s="374"/>
+      <c r="B53" s="375"/>
+      <c r="C53" s="375"/>
+      <c r="D53" s="376"/>
       <c r="E53" s="128" t="s">
         <v>344</v>
       </c>
@@ -14712,18 +14715,18 @@
       <c r="H53" s="101">
         <v>1</v>
       </c>
-      <c r="I53" s="369" t="s">
+      <c r="I53" s="364" t="s">
         <v>345</v>
       </c>
-      <c r="J53" s="369"/>
-      <c r="K53" s="370"/>
+      <c r="J53" s="364"/>
+      <c r="K53" s="365"/>
     </row>
     <row r="54" spans="1:11" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="401" t="s">
+      <c r="A54" s="367" t="s">
         <v>346</v>
       </c>
-      <c r="B54" s="402"/>
-      <c r="C54" s="402"/>
+      <c r="B54" s="347"/>
+      <c r="C54" s="347"/>
       <c r="D54" s="122" t="s">
         <v>347</v>
       </c>
@@ -14739,18 +14742,18 @@
       <c r="H54" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I54" s="419" t="s">
+      <c r="I54" s="368" t="s">
         <v>349</v>
       </c>
-      <c r="J54" s="419"/>
-      <c r="K54" s="420"/>
+      <c r="J54" s="368"/>
+      <c r="K54" s="369"/>
     </row>
     <row r="55" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="401" t="s">
+      <c r="A55" s="367" t="s">
         <v>350</v>
       </c>
-      <c r="B55" s="402"/>
-      <c r="C55" s="402"/>
+      <c r="B55" s="347"/>
+      <c r="C55" s="347"/>
       <c r="D55" s="122" t="s">
         <v>351</v>
       </c>
@@ -14766,18 +14769,18 @@
       <c r="H55" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I55" s="419" t="s">
+      <c r="I55" s="368" t="s">
         <v>353</v>
       </c>
-      <c r="J55" s="419"/>
-      <c r="K55" s="420"/>
+      <c r="J55" s="368"/>
+      <c r="K55" s="369"/>
     </row>
     <row r="56" spans="1:11" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="403" t="s">
+      <c r="A56" s="373" t="s">
         <v>354</v>
       </c>
-      <c r="B56" s="404"/>
-      <c r="C56" s="404"/>
+      <c r="B56" s="366"/>
+      <c r="C56" s="366"/>
       <c r="D56" s="122" t="s">
         <v>355</v>
       </c>
@@ -14793,18 +14796,18 @@
       <c r="H56" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="I56" s="421" t="s">
+      <c r="I56" s="370" t="s">
         <v>358</v>
       </c>
-      <c r="J56" s="422"/>
-      <c r="K56" s="423"/>
+      <c r="J56" s="371"/>
+      <c r="K56" s="372"/>
     </row>
     <row r="57" spans="1:11" ht="261" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="405" t="s">
+      <c r="A57" s="374" t="s">
         <v>359</v>
       </c>
-      <c r="B57" s="406"/>
-      <c r="C57" s="406"/>
+      <c r="B57" s="375"/>
+      <c r="C57" s="375"/>
       <c r="D57" s="108" t="s">
         <v>360</v>
       </c>
@@ -14820,18 +14823,18 @@
       <c r="H57" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="I57" s="421" t="s">
+      <c r="I57" s="370" t="s">
         <v>363</v>
       </c>
-      <c r="J57" s="422"/>
-      <c r="K57" s="423"/>
+      <c r="J57" s="371"/>
+      <c r="K57" s="372"/>
     </row>
     <row r="58" spans="1:11" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="401" t="s">
+      <c r="A58" s="367" t="s">
         <v>364</v>
       </c>
-      <c r="B58" s="402"/>
-      <c r="C58" s="402"/>
+      <c r="B58" s="347"/>
+      <c r="C58" s="347"/>
       <c r="D58" s="91" t="s">
         <v>365</v>
       </c>
@@ -14847,18 +14850,18 @@
       <c r="H58" s="33">
         <v>1</v>
       </c>
-      <c r="I58" s="424" t="s">
+      <c r="I58" s="352" t="s">
         <v>366</v>
       </c>
-      <c r="J58" s="424"/>
-      <c r="K58" s="425"/>
+      <c r="J58" s="352"/>
+      <c r="K58" s="353"/>
     </row>
     <row r="59" spans="1:11" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="401" t="s">
+      <c r="A59" s="367" t="s">
         <v>367</v>
       </c>
-      <c r="B59" s="402"/>
-      <c r="C59" s="402"/>
+      <c r="B59" s="347"/>
+      <c r="C59" s="347"/>
       <c r="D59" s="122" t="s">
         <v>368</v>
       </c>
@@ -14874,18 +14877,18 @@
       <c r="H59" s="34">
         <v>3</v>
       </c>
-      <c r="I59" s="424" t="s">
+      <c r="I59" s="352" t="s">
         <v>133</v>
       </c>
-      <c r="J59" s="424"/>
-      <c r="K59" s="425"/>
+      <c r="J59" s="352"/>
+      <c r="K59" s="353"/>
     </row>
     <row r="60" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="403" t="s">
+      <c r="A60" s="373" t="s">
         <v>369</v>
       </c>
-      <c r="B60" s="404"/>
-      <c r="C60" s="404"/>
+      <c r="B60" s="366"/>
+      <c r="C60" s="366"/>
       <c r="D60" s="122" t="s">
         <v>370</v>
       </c>
@@ -14901,18 +14904,18 @@
       <c r="H60" s="89" t="s">
         <v>191</v>
       </c>
-      <c r="I60" s="359" t="s">
+      <c r="I60" s="350" t="s">
         <v>146</v>
       </c>
-      <c r="J60" s="359"/>
-      <c r="K60" s="360"/>
+      <c r="J60" s="350"/>
+      <c r="K60" s="351"/>
     </row>
     <row r="61" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A61" s="403" t="s">
+      <c r="A61" s="373" t="s">
         <v>371</v>
       </c>
-      <c r="B61" s="404"/>
-      <c r="C61" s="404"/>
+      <c r="B61" s="366"/>
+      <c r="C61" s="366"/>
       <c r="D61" s="122" t="s">
         <v>372</v>
       </c>
@@ -14928,60 +14931,60 @@
       <c r="H61" s="87">
         <v>1</v>
       </c>
-      <c r="I61" s="369" t="s">
+      <c r="I61" s="364" t="s">
         <v>374</v>
       </c>
-      <c r="J61" s="369"/>
-      <c r="K61" s="370"/>
+      <c r="J61" s="364"/>
+      <c r="K61" s="365"/>
     </row>
     <row r="62" spans="1:11" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="428" t="s">
+      <c r="A62" s="354" t="s">
         <v>375</v>
       </c>
-      <c r="B62" s="429"/>
-      <c r="C62" s="430"/>
+      <c r="B62" s="355"/>
+      <c r="C62" s="356"/>
       <c r="D62" s="121" t="s">
         <v>376</v>
       </c>
-      <c r="E62" s="364" t="s">
+      <c r="E62" s="433" t="s">
         <v>377</v>
       </c>
-      <c r="F62" s="365" t="s">
+      <c r="F62" s="434" t="s">
         <v>12</v>
       </c>
-      <c r="G62" s="365" t="s">
+      <c r="G62" s="434" t="s">
         <v>24</v>
       </c>
-      <c r="H62" s="366">
+      <c r="H62" s="435">
         <v>1</v>
       </c>
-      <c r="I62" s="359" t="s">
+      <c r="I62" s="350" t="s">
         <v>378</v>
       </c>
-      <c r="J62" s="359"/>
-      <c r="K62" s="360"/>
+      <c r="J62" s="350"/>
+      <c r="K62" s="351"/>
     </row>
     <row r="63" spans="1:11" ht="180.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="431"/>
-      <c r="B63" s="432"/>
-      <c r="C63" s="433"/>
+      <c r="A63" s="357"/>
+      <c r="B63" s="358"/>
+      <c r="C63" s="359"/>
       <c r="D63" s="125" t="s">
         <v>379</v>
       </c>
-      <c r="E63" s="364"/>
-      <c r="F63" s="365"/>
-      <c r="G63" s="365"/>
-      <c r="H63" s="366"/>
-      <c r="I63" s="367"/>
-      <c r="J63" s="367"/>
-      <c r="K63" s="368"/>
+      <c r="E63" s="433"/>
+      <c r="F63" s="434"/>
+      <c r="G63" s="434"/>
+      <c r="H63" s="435"/>
+      <c r="I63" s="436"/>
+      <c r="J63" s="436"/>
+      <c r="K63" s="437"/>
     </row>
     <row r="64" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="434" t="s">
+      <c r="A64" s="360" t="s">
         <v>380</v>
       </c>
-      <c r="B64" s="435"/>
-      <c r="C64" s="435"/>
+      <c r="B64" s="361"/>
+      <c r="C64" s="361"/>
       <c r="D64" s="125" t="s">
         <v>381</v>
       </c>
@@ -14997,16 +15000,16 @@
       <c r="H64" s="138">
         <v>2</v>
       </c>
-      <c r="I64" s="359" t="s">
+      <c r="I64" s="350" t="s">
         <v>383</v>
       </c>
-      <c r="J64" s="359"/>
-      <c r="K64" s="360"/>
+      <c r="J64" s="350"/>
+      <c r="K64" s="351"/>
     </row>
     <row r="65" spans="1:11" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="436"/>
-      <c r="B65" s="437"/>
-      <c r="C65" s="437"/>
+      <c r="A65" s="362"/>
+      <c r="B65" s="363"/>
+      <c r="C65" s="363"/>
       <c r="D65" s="130" t="s">
         <v>384</v>
       </c>
@@ -15022,18 +15025,18 @@
       <c r="H65" s="139">
         <v>3</v>
       </c>
-      <c r="I65" s="359" t="s">
+      <c r="I65" s="350" t="s">
         <v>386</v>
       </c>
-      <c r="J65" s="359"/>
-      <c r="K65" s="360"/>
+      <c r="J65" s="350"/>
+      <c r="K65" s="351"/>
     </row>
     <row r="66" spans="1:11" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="401" t="s">
+      <c r="A66" s="367" t="s">
         <v>387</v>
       </c>
-      <c r="B66" s="402"/>
-      <c r="C66" s="402"/>
+      <c r="B66" s="347"/>
+      <c r="C66" s="347"/>
       <c r="D66" s="131" t="s">
         <v>388</v>
       </c>
@@ -15049,18 +15052,18 @@
       <c r="H66" s="139" t="s">
         <v>192</v>
       </c>
-      <c r="I66" s="359" t="s">
+      <c r="I66" s="350" t="s">
         <v>390</v>
       </c>
-      <c r="J66" s="359"/>
-      <c r="K66" s="360"/>
+      <c r="J66" s="350"/>
+      <c r="K66" s="351"/>
     </row>
     <row r="67" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="401" t="s">
+      <c r="A67" s="367" t="s">
         <v>391</v>
       </c>
-      <c r="B67" s="402"/>
-      <c r="C67" s="402"/>
+      <c r="B67" s="347"/>
+      <c r="C67" s="347"/>
       <c r="D67" s="91" t="s">
         <v>392</v>
       </c>
@@ -15076,18 +15079,18 @@
       <c r="H67" s="140">
         <v>8</v>
       </c>
-      <c r="I67" s="359" t="s">
+      <c r="I67" s="350" t="s">
         <v>394</v>
       </c>
-      <c r="J67" s="359"/>
-      <c r="K67" s="360"/>
+      <c r="J67" s="350"/>
+      <c r="K67" s="351"/>
     </row>
     <row r="68" spans="1:11" ht="57" x14ac:dyDescent="0.25">
-      <c r="A68" s="407" t="s">
+      <c r="A68" s="385" t="s">
         <v>395</v>
       </c>
-      <c r="B68" s="408"/>
-      <c r="C68" s="409"/>
+      <c r="B68" s="386"/>
+      <c r="C68" s="387"/>
       <c r="D68" s="122" t="s">
         <v>396</v>
       </c>
@@ -15103,37 +15106,37 @@
       <c r="H68" s="139" t="s">
         <v>143</v>
       </c>
-      <c r="I68" s="359" t="s">
+      <c r="I68" s="350" t="s">
         <v>398</v>
       </c>
-      <c r="J68" s="359"/>
-      <c r="K68" s="360"/>
+      <c r="J68" s="350"/>
+      <c r="K68" s="351"/>
     </row>
     <row r="69" spans="1:11" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="402" t="s">
+      <c r="A69" s="347" t="s">
         <v>399</v>
       </c>
-      <c r="B69" s="402"/>
-      <c r="C69" s="402"/>
+      <c r="B69" s="347"/>
+      <c r="C69" s="347"/>
       <c r="D69" s="142" t="s">
         <v>400</v>
       </c>
-      <c r="E69" s="361" t="s">
+      <c r="E69" s="430" t="s">
         <v>401</v>
       </c>
-      <c r="F69" s="362"/>
-      <c r="G69" s="362"/>
-      <c r="H69" s="362"/>
-      <c r="I69" s="362"/>
-      <c r="J69" s="362"/>
-      <c r="K69" s="363"/>
+      <c r="F69" s="431"/>
+      <c r="G69" s="431"/>
+      <c r="H69" s="431"/>
+      <c r="I69" s="431"/>
+      <c r="J69" s="431"/>
+      <c r="K69" s="432"/>
     </row>
     <row r="70" spans="1:11" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="402" t="s">
+      <c r="A70" s="347" t="s">
         <v>402</v>
       </c>
-      <c r="B70" s="402"/>
-      <c r="C70" s="402"/>
+      <c r="B70" s="347"/>
+      <c r="C70" s="347"/>
       <c r="D70" s="121" t="s">
         <v>403</v>
       </c>
@@ -15149,18 +15152,18 @@
       <c r="H70" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="I70" s="359" t="s">
+      <c r="I70" s="350" t="s">
         <v>406</v>
       </c>
-      <c r="J70" s="359"/>
-      <c r="K70" s="359"/>
+      <c r="J70" s="350"/>
+      <c r="K70" s="350"/>
     </row>
     <row r="71" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="404" t="s">
+      <c r="A71" s="366" t="s">
         <v>407</v>
       </c>
-      <c r="B71" s="404"/>
-      <c r="C71" s="404"/>
+      <c r="B71" s="366"/>
+      <c r="C71" s="366"/>
       <c r="D71" s="122" t="s">
         <v>408</v>
       </c>
@@ -15176,37 +15179,37 @@
       <c r="H71" s="87" t="s">
         <v>410</v>
       </c>
-      <c r="I71" s="359" t="s">
+      <c r="I71" s="350" t="s">
         <v>411</v>
       </c>
-      <c r="J71" s="359"/>
-      <c r="K71" s="359"/>
+      <c r="J71" s="350"/>
+      <c r="K71" s="350"/>
     </row>
     <row r="72" spans="1:11" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="402" t="s">
+      <c r="A72" s="347" t="s">
         <v>412</v>
       </c>
-      <c r="B72" s="402"/>
-      <c r="C72" s="402"/>
+      <c r="B72" s="347"/>
+      <c r="C72" s="347"/>
       <c r="D72" s="142" t="s">
         <v>413</v>
       </c>
-      <c r="E72" s="347" t="s">
+      <c r="E72" s="418" t="s">
         <v>401</v>
       </c>
-      <c r="F72" s="348"/>
-      <c r="G72" s="348"/>
-      <c r="H72" s="348"/>
-      <c r="I72" s="348"/>
-      <c r="J72" s="348"/>
-      <c r="K72" s="349"/>
+      <c r="F72" s="419"/>
+      <c r="G72" s="419"/>
+      <c r="H72" s="419"/>
+      <c r="I72" s="419"/>
+      <c r="J72" s="419"/>
+      <c r="K72" s="420"/>
     </row>
     <row r="73" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="402" t="s">
+      <c r="A73" s="347" t="s">
         <v>414</v>
       </c>
-      <c r="B73" s="402"/>
-      <c r="C73" s="402"/>
+      <c r="B73" s="347"/>
+      <c r="C73" s="347"/>
       <c r="D73" s="122" t="s">
         <v>415</v>
       </c>
@@ -15222,37 +15225,37 @@
       <c r="H73" s="87">
         <v>3</v>
       </c>
-      <c r="I73" s="350" t="s">
+      <c r="I73" s="421" t="s">
         <v>417</v>
       </c>
-      <c r="J73" s="351"/>
-      <c r="K73" s="352"/>
+      <c r="J73" s="422"/>
+      <c r="K73" s="423"/>
     </row>
     <row r="74" spans="1:11" ht="300.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="402" t="s">
+      <c r="A74" s="347" t="s">
         <v>418</v>
       </c>
-      <c r="B74" s="402"/>
-      <c r="C74" s="402"/>
+      <c r="B74" s="347"/>
+      <c r="C74" s="347"/>
       <c r="D74" s="121" t="s">
         <v>419</v>
       </c>
-      <c r="E74" s="356" t="s">
+      <c r="E74" s="427" t="s">
         <v>401</v>
       </c>
-      <c r="F74" s="357"/>
-      <c r="G74" s="357"/>
-      <c r="H74" s="357"/>
-      <c r="I74" s="357"/>
-      <c r="J74" s="357"/>
-      <c r="K74" s="358"/>
+      <c r="F74" s="428"/>
+      <c r="G74" s="428"/>
+      <c r="H74" s="428"/>
+      <c r="I74" s="428"/>
+      <c r="J74" s="428"/>
+      <c r="K74" s="429"/>
     </row>
     <row r="75" spans="1:11" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="426" t="s">
+      <c r="A75" s="348" t="s">
         <v>420</v>
       </c>
-      <c r="B75" s="427"/>
-      <c r="C75" s="427"/>
+      <c r="B75" s="349"/>
+      <c r="C75" s="349"/>
       <c r="D75" s="143" t="s">
         <v>421</v>
       </c>
@@ -15268,11 +15271,11 @@
       <c r="H75" s="146">
         <v>7</v>
       </c>
-      <c r="I75" s="353" t="s">
+      <c r="I75" s="424" t="s">
         <v>423</v>
       </c>
-      <c r="J75" s="354"/>
-      <c r="K75" s="355"/>
+      <c r="J75" s="425"/>
+      <c r="K75" s="426"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="89">
@@ -15401,6 +15404,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="E72:K72"/>
+    <mergeCell ref="I73:K73"/>
+    <mergeCell ref="I75:K75"/>
+    <mergeCell ref="E74:K74"/>
+    <mergeCell ref="E49:K49"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="E69:K69"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="I62:K63"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="E25:P25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="D17:P17"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="E18:P18"/>
+    <mergeCell ref="E19:P19"/>
+    <mergeCell ref="E20:P20"/>
+    <mergeCell ref="E21:P21"/>
+    <mergeCell ref="E23:P23"/>
+    <mergeCell ref="E24:P24"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="E15:P15"/>
+    <mergeCell ref="E16:P16"/>
+    <mergeCell ref="E22:P22"/>
+    <mergeCell ref="E31:K31"/>
+    <mergeCell ref="E32:K32"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:K33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:K34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:K35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:K36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:K37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:K40"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:K38"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
     <mergeCell ref="A74:C74"/>
     <mergeCell ref="A75:C75"/>
     <mergeCell ref="I66:K66"/>
@@ -15417,82 +15496,6 @@
     <mergeCell ref="A72:C72"/>
     <mergeCell ref="A73:C73"/>
     <mergeCell ref="A66:C66"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:K37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:K39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="E40:K40"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E38:K38"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="E34:K34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:K35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:K36"/>
-    <mergeCell ref="E31:K31"/>
-    <mergeCell ref="E32:K32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:K33"/>
-    <mergeCell ref="E25:P25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="D17:P17"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="E18:P18"/>
-    <mergeCell ref="E19:P19"/>
-    <mergeCell ref="E20:P20"/>
-    <mergeCell ref="E21:P21"/>
-    <mergeCell ref="E23:P23"/>
-    <mergeCell ref="E24:P24"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="E15:P15"/>
-    <mergeCell ref="E16:P16"/>
-    <mergeCell ref="E22:P22"/>
-    <mergeCell ref="E72:K72"/>
-    <mergeCell ref="I73:K73"/>
-    <mergeCell ref="I75:K75"/>
-    <mergeCell ref="E74:K74"/>
-    <mergeCell ref="E49:K49"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="E69:K69"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="I62:K63"/>
-    <mergeCell ref="I53:K53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18280,7 +18283,7 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
@@ -18942,19 +18945,19 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="440">
+      <c r="A4" s="445">
         <v>0.1</v>
       </c>
       <c r="B4" s="251" t="s">
         <v>1144</v>
       </c>
-      <c r="C4" s="449" t="s">
+      <c r="C4" s="438" t="s">
         <v>1145</v>
       </c>
-      <c r="D4" s="449" t="s">
+      <c r="D4" s="438" t="s">
         <v>1146</v>
       </c>
-      <c r="E4" s="446" t="s">
+      <c r="E4" s="439" t="s">
         <v>1147</v>
       </c>
       <c r="F4" s="272" t="s">
@@ -18971,13 +18974,13 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="440"/>
+      <c r="A5" s="445"/>
       <c r="B5" t="s">
         <v>1151</v>
       </c>
-      <c r="C5" s="449"/>
-      <c r="D5" s="449"/>
-      <c r="E5" s="446"/>
+      <c r="C5" s="438"/>
+      <c r="D5" s="438"/>
+      <c r="E5" s="439"/>
       <c r="F5" t="s">
         <v>1152</v>
       </c>
@@ -18992,48 +18995,48 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="440"/>
+      <c r="A6" s="445"/>
       <c r="B6" t="s">
         <v>1155</v>
       </c>
-      <c r="C6" s="449"/>
-      <c r="D6" s="449"/>
-      <c r="E6" s="446"/>
+      <c r="C6" s="438"/>
+      <c r="D6" s="438"/>
+      <c r="E6" s="439"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="440"/>
+      <c r="A7" s="445"/>
       <c r="B7" t="s">
         <v>1156</v>
       </c>
-      <c r="C7" s="449"/>
-      <c r="D7" s="449"/>
-      <c r="E7" s="446"/>
+      <c r="C7" s="438"/>
+      <c r="D7" s="438"/>
+      <c r="E7" s="439"/>
       <c r="F7" s="272"/>
       <c r="G7" s="188"/>
       <c r="H7" s="271"/>
       <c r="I7" s="188"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="440"/>
+      <c r="A8" s="445"/>
       <c r="B8" s="223" t="s">
         <v>1157</v>
       </c>
-      <c r="C8" s="449"/>
-      <c r="D8" s="449"/>
-      <c r="E8" s="446"/>
+      <c r="C8" s="438"/>
+      <c r="D8" s="438"/>
+      <c r="E8" s="439"/>
       <c r="F8" s="272"/>
       <c r="G8" s="188"/>
       <c r="H8" s="271"/>
       <c r="I8" s="188"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="440"/>
+      <c r="A9" s="445"/>
       <c r="B9" t="s">
         <v>1158</v>
       </c>
-      <c r="C9" s="449"/>
-      <c r="D9" s="449"/>
-      <c r="E9" s="446"/>
+      <c r="C9" s="438"/>
+      <c r="D9" s="438"/>
+      <c r="E9" s="439"/>
       <c r="G9" s="188"/>
       <c r="H9" s="271"/>
       <c r="I9" s="277" t="s">
@@ -19041,13 +19044,13 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="440"/>
+      <c r="A10" s="445"/>
       <c r="B10" s="223" t="s">
         <v>1160</v>
       </c>
-      <c r="C10" s="449"/>
-      <c r="D10" s="449"/>
-      <c r="E10" s="446"/>
+      <c r="C10" s="438"/>
+      <c r="D10" s="438"/>
+      <c r="E10" s="439"/>
       <c r="F10" s="272"/>
       <c r="G10" s="188"/>
       <c r="H10" s="271"/>
@@ -19056,82 +19059,82 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="440"/>
+      <c r="A11" s="445"/>
       <c r="B11" t="s">
         <v>1162</v>
       </c>
-      <c r="C11" s="449"/>
-      <c r="D11" s="449"/>
-      <c r="E11" s="446"/>
+      <c r="C11" s="438"/>
+      <c r="D11" s="438"/>
+      <c r="E11" s="439"/>
       <c r="F11" s="272"/>
       <c r="G11" s="188"/>
       <c r="H11" s="271"/>
       <c r="I11" s="188"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="440"/>
+      <c r="A12" s="445"/>
       <c r="B12" t="s">
         <v>1163</v>
       </c>
-      <c r="C12" s="449"/>
-      <c r="D12" s="449"/>
-      <c r="E12" s="446"/>
+      <c r="C12" s="438"/>
+      <c r="D12" s="438"/>
+      <c r="E12" s="439"/>
       <c r="F12" s="272"/>
       <c r="G12" s="188"/>
       <c r="H12" s="271"/>
       <c r="I12" s="188"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="440"/>
+      <c r="A13" s="445"/>
       <c r="B13" t="s">
         <v>1164</v>
       </c>
-      <c r="C13" s="449"/>
-      <c r="D13" s="449"/>
-      <c r="E13" s="446"/>
+      <c r="C13" s="438"/>
+      <c r="D13" s="438"/>
+      <c r="E13" s="439"/>
       <c r="F13" s="272"/>
       <c r="G13" s="188"/>
       <c r="H13" s="271"/>
       <c r="I13" s="188"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="440"/>
+      <c r="A14" s="445"/>
       <c r="B14" t="s">
         <v>1165</v>
       </c>
-      <c r="C14" s="449"/>
-      <c r="D14" s="449"/>
-      <c r="E14" s="446"/>
+      <c r="C14" s="438"/>
+      <c r="D14" s="438"/>
+      <c r="E14" s="439"/>
       <c r="F14" s="272"/>
       <c r="G14" s="188"/>
       <c r="H14" s="271"/>
       <c r="I14" s="188"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="440"/>
+      <c r="A15" s="445"/>
       <c r="B15" t="s">
         <v>1166</v>
       </c>
-      <c r="C15" s="449"/>
-      <c r="D15" s="449"/>
-      <c r="E15" s="446"/>
+      <c r="C15" s="438"/>
+      <c r="D15" s="438"/>
+      <c r="E15" s="439"/>
       <c r="F15" s="272"/>
       <c r="G15" s="188"/>
       <c r="H15" s="271"/>
       <c r="I15" s="188"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="441">
+      <c r="A16" s="446">
         <v>0.2</v>
       </c>
       <c r="B16" s="252" t="s">
         <v>1167</v>
       </c>
-      <c r="C16" s="449" t="s">
+      <c r="C16" s="438" t="s">
         <v>1168</v>
       </c>
-      <c r="D16" s="446"/>
-      <c r="E16" s="447" t="s">
+      <c r="D16" s="439"/>
+      <c r="E16" s="440" t="s">
         <v>1147</v>
       </c>
       <c r="F16" t="s">
@@ -19142,126 +19145,126 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="441"/>
+      <c r="A17" s="446"/>
       <c r="B17" s="223" t="s">
         <v>1170</v>
       </c>
-      <c r="C17" s="449"/>
-      <c r="D17" s="446"/>
-      <c r="E17" s="447"/>
+      <c r="C17" s="438"/>
+      <c r="D17" s="439"/>
+      <c r="E17" s="440"/>
       <c r="F17" t="s">
         <v>1171</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="441"/>
+      <c r="A18" s="446"/>
       <c r="B18" t="s">
         <v>1172</v>
       </c>
-      <c r="C18" s="449"/>
-      <c r="D18" s="446"/>
-      <c r="E18" s="447"/>
+      <c r="C18" s="438"/>
+      <c r="D18" s="439"/>
+      <c r="E18" s="440"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="441"/>
+      <c r="A19" s="446"/>
       <c r="B19" t="s">
         <v>1173</v>
       </c>
-      <c r="C19" s="449"/>
-      <c r="D19" s="446"/>
-      <c r="E19" s="447"/>
+      <c r="C19" s="438"/>
+      <c r="D19" s="439"/>
+      <c r="E19" s="440"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="441"/>
+      <c r="A20" s="446"/>
       <c r="B20" t="s">
         <v>1174</v>
       </c>
-      <c r="C20" s="449"/>
-      <c r="D20" s="446"/>
-      <c r="E20" s="447"/>
+      <c r="C20" s="438"/>
+      <c r="D20" s="439"/>
+      <c r="E20" s="440"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="441"/>
+      <c r="A21" s="446"/>
       <c r="B21" t="s">
         <v>1175</v>
       </c>
-      <c r="C21" s="449"/>
-      <c r="D21" s="446"/>
-      <c r="E21" s="447"/>
+      <c r="C21" s="438"/>
+      <c r="D21" s="439"/>
+      <c r="E21" s="440"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="441"/>
+      <c r="A22" s="446"/>
       <c r="B22" s="223" t="s">
         <v>1176</v>
       </c>
-      <c r="C22" s="449"/>
-      <c r="D22" s="446"/>
-      <c r="E22" s="447"/>
+      <c r="C22" s="438"/>
+      <c r="D22" s="439"/>
+      <c r="E22" s="440"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="441"/>
+      <c r="A23" s="446"/>
       <c r="B23" s="223" t="s">
         <v>1177</v>
       </c>
-      <c r="C23" s="449"/>
-      <c r="D23" s="446"/>
-      <c r="E23" s="447"/>
+      <c r="C23" s="438"/>
+      <c r="D23" s="439"/>
+      <c r="E23" s="440"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="441"/>
+      <c r="A24" s="446"/>
       <c r="B24" t="s">
         <v>1178</v>
       </c>
-      <c r="C24" s="449"/>
-      <c r="D24" s="446"/>
-      <c r="E24" s="447"/>
+      <c r="C24" s="438"/>
+      <c r="D24" s="439"/>
+      <c r="E24" s="440"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="441"/>
+      <c r="A25" s="446"/>
       <c r="B25" t="s">
         <v>1179</v>
       </c>
-      <c r="C25" s="449"/>
-      <c r="D25" s="446"/>
-      <c r="E25" s="447"/>
+      <c r="C25" s="438"/>
+      <c r="D25" s="439"/>
+      <c r="E25" s="440"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="441"/>
+      <c r="A26" s="446"/>
       <c r="B26" t="s">
         <v>1180</v>
       </c>
-      <c r="C26" s="449"/>
-      <c r="D26" s="446"/>
-      <c r="E26" s="447"/>
+      <c r="C26" s="438"/>
+      <c r="D26" s="439"/>
+      <c r="E26" s="440"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="441"/>
+      <c r="A27" s="446"/>
       <c r="B27" t="s">
         <v>1181</v>
       </c>
-      <c r="C27" s="449"/>
-      <c r="D27" s="446"/>
-      <c r="E27" s="447"/>
+      <c r="C27" s="438"/>
+      <c r="D27" s="439"/>
+      <c r="E27" s="440"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="441"/>
+      <c r="A28" s="446"/>
       <c r="B28" t="s">
         <v>1182</v>
       </c>
-      <c r="C28" s="449"/>
-      <c r="D28" s="446"/>
-      <c r="E28" s="447"/>
+      <c r="C28" s="438"/>
+      <c r="D28" s="439"/>
+      <c r="E28" s="440"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="442">
+      <c r="A29" s="447">
         <v>0.3</v>
       </c>
       <c r="B29" s="256" t="s">
         <v>1183</v>
       </c>
-      <c r="C29" s="445"/>
-      <c r="D29" s="448"/>
-      <c r="E29" s="446" t="s">
+      <c r="C29" s="441"/>
+      <c r="D29" s="442"/>
+      <c r="E29" s="439" t="s">
         <v>1147</v>
       </c>
       <c r="H29" s="274" t="s">
@@ -19269,52 +19272,52 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="442"/>
+      <c r="A30" s="447"/>
       <c r="B30" s="223" t="s">
         <v>1184</v>
       </c>
-      <c r="C30" s="445"/>
-      <c r="D30" s="448"/>
-      <c r="E30" s="446"/>
+      <c r="C30" s="441"/>
+      <c r="D30" s="442"/>
+      <c r="E30" s="439"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="442"/>
+      <c r="A31" s="447"/>
       <c r="B31" t="s">
         <v>1185</v>
       </c>
-      <c r="C31" s="445"/>
-      <c r="D31" s="448"/>
-      <c r="E31" s="446"/>
+      <c r="C31" s="441"/>
+      <c r="D31" s="442"/>
+      <c r="E31" s="439"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="442"/>
+      <c r="A32" s="447"/>
       <c r="B32" s="265" t="s">
         <v>1186</v>
       </c>
-      <c r="C32" s="445"/>
-      <c r="D32" s="448"/>
-      <c r="E32" s="446"/>
+      <c r="C32" s="441"/>
+      <c r="D32" s="442"/>
+      <c r="E32" s="439"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="442"/>
+      <c r="A33" s="447"/>
       <c r="B33" t="s">
         <v>1187</v>
       </c>
-      <c r="C33" s="445"/>
-      <c r="D33" s="448"/>
-      <c r="E33" s="446"/>
+      <c r="C33" s="441"/>
+      <c r="D33" s="442"/>
+      <c r="E33" s="439"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="442"/>
+      <c r="A34" s="447"/>
       <c r="B34" t="s">
         <v>1188</v>
       </c>
-      <c r="C34" s="445"/>
-      <c r="D34" s="448"/>
-      <c r="E34" s="446"/>
+      <c r="C34" s="441"/>
+      <c r="D34" s="442"/>
+      <c r="E34" s="439"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="443">
+      <c r="A35" s="448">
         <v>1.1000000000000001</v>
       </c>
       <c r="B35" s="260" t="s">
@@ -19323,7 +19326,7 @@
       <c r="C35" s="257" t="s">
         <v>1190</v>
       </c>
-      <c r="E35" s="446" t="s">
+      <c r="E35" s="439" t="s">
         <v>1191</v>
       </c>
       <c r="G35" t="s">
@@ -19334,11 +19337,11 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="443"/>
+      <c r="A36" s="448"/>
       <c r="B36" s="223" t="s">
         <v>1193</v>
       </c>
-      <c r="E36" s="446"/>
+      <c r="E36" s="439"/>
       <c r="F36" s="272" t="s">
         <v>1194</v>
       </c>
@@ -19353,11 +19356,11 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="443"/>
+      <c r="A37" s="448"/>
       <c r="B37" t="s">
         <v>1197</v>
       </c>
-      <c r="E37" s="446"/>
+      <c r="E37" s="439"/>
       <c r="F37" s="272" t="s">
         <v>1198</v>
       </c>
@@ -19372,62 +19375,62 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="443"/>
+      <c r="A38" s="448"/>
       <c r="B38" t="s">
         <v>1201</v>
       </c>
-      <c r="E38" s="446"/>
+      <c r="E38" s="439"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="443"/>
+      <c r="A39" s="448"/>
       <c r="B39" t="s">
         <v>1202</v>
       </c>
-      <c r="E39" s="446"/>
+      <c r="E39" s="439"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="443"/>
+      <c r="A40" s="448"/>
       <c r="B40" t="s">
         <v>1203</v>
       </c>
-      <c r="E40" s="446"/>
+      <c r="E40" s="439"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="443"/>
+      <c r="A41" s="448"/>
       <c r="B41" t="s">
         <v>1204</v>
       </c>
-      <c r="E41" s="446"/>
+      <c r="E41" s="439"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="443"/>
+      <c r="A42" s="448"/>
       <c r="B42" t="s">
         <v>1205</v>
       </c>
-      <c r="E42" s="446"/>
+      <c r="E42" s="439"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="443"/>
+      <c r="A43" s="448"/>
       <c r="B43" t="s">
         <v>1206</v>
       </c>
-      <c r="E43" s="446"/>
+      <c r="E43" s="439"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="443"/>
+      <c r="A44" s="448"/>
       <c r="B44" t="s">
         <v>1207</v>
       </c>
-      <c r="E44" s="446"/>
+      <c r="E44" s="439"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="444">
+      <c r="A47" s="449">
         <v>1.2</v>
       </c>
       <c r="B47" s="262" t="s">
         <v>1208</v>
       </c>
-      <c r="E47" s="446" t="s">
+      <c r="E47" s="439" t="s">
         <v>1209</v>
       </c>
       <c r="G47" t="s">
@@ -19438,35 +19441,35 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="444"/>
+      <c r="A48" s="449"/>
       <c r="B48" s="223" t="s">
         <v>1211</v>
       </c>
-      <c r="E48" s="446"/>
+      <c r="E48" s="439"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="444"/>
+      <c r="A49" s="449"/>
       <c r="B49" s="223" t="s">
         <v>1212</v>
       </c>
-      <c r="E49" s="446"/>
+      <c r="E49" s="439"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="444"/>
+      <c r="A50" s="449"/>
       <c r="B50" t="s">
         <v>1213</v>
       </c>
-      <c r="E50" s="446"/>
+      <c r="E50" s="439"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="444"/>
+      <c r="A51" s="449"/>
       <c r="B51" t="s">
         <v>1206</v>
       </c>
-      <c r="E51" s="446"/>
+      <c r="E51" s="439"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="438">
+      <c r="A54" s="443">
         <v>1.3</v>
       </c>
       <c r="B54" s="264" t="s">
@@ -19478,7 +19481,7 @@
       <c r="D54" t="s">
         <v>1216</v>
       </c>
-      <c r="E54" s="447" t="s">
+      <c r="E54" s="440" t="s">
         <v>1217</v>
       </c>
       <c r="G54" t="s">
@@ -19492,41 +19495,41 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="438"/>
+      <c r="A55" s="443"/>
       <c r="B55" s="223" t="s">
         <v>1220</v>
       </c>
-      <c r="E55" s="447"/>
+      <c r="E55" s="440"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="438"/>
+      <c r="A56" s="443"/>
       <c r="B56" t="s">
         <v>1221</v>
       </c>
-      <c r="E56" s="447"/>
+      <c r="E56" s="440"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="438"/>
+      <c r="A57" s="443"/>
       <c r="B57" t="s">
         <v>1222</v>
       </c>
-      <c r="E57" s="447"/>
+      <c r="E57" s="440"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="438"/>
+      <c r="A58" s="443"/>
       <c r="B58" t="s">
         <v>1223</v>
       </c>
-      <c r="E58" s="447"/>
+      <c r="E58" s="440"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="439">
+      <c r="A61" s="444">
         <v>1.4</v>
       </c>
       <c r="B61" s="267" t="s">
         <v>1224</v>
       </c>
-      <c r="E61" s="447" t="s">
+      <c r="E61" s="440" t="s">
         <v>1225</v>
       </c>
       <c r="G61" t="s">
@@ -19537,38 +19540,38 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="439"/>
+      <c r="A62" s="444"/>
       <c r="B62" s="223" t="s">
         <v>1227</v>
       </c>
-      <c r="E62" s="447"/>
+      <c r="E62" s="440"/>
       <c r="G62" s="257" t="s">
         <v>1228</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="439"/>
+      <c r="A63" s="444"/>
       <c r="B63" t="s">
         <v>1229</v>
       </c>
-      <c r="E63" s="447"/>
+      <c r="E63" s="440"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="439"/>
+      <c r="A64" s="444"/>
       <c r="B64" t="s">
         <v>1230</v>
       </c>
-      <c r="E64" s="447"/>
+      <c r="E64" s="440"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="439"/>
+      <c r="A65" s="444"/>
       <c r="B65" t="s">
         <v>1231</v>
       </c>
-      <c r="E65" s="447"/>
+      <c r="E65" s="440"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="440">
+      <c r="A67" s="445">
         <v>1.5</v>
       </c>
       <c r="B67" s="251" t="s">
@@ -19579,19 +19582,19 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="440"/>
+      <c r="A68" s="445"/>
       <c r="B68" s="223" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="440"/>
+      <c r="A69" s="445"/>
       <c r="B69" t="s">
         <v>1234</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="441">
+      <c r="A72" s="446">
         <v>1.6</v>
       </c>
       <c r="B72" s="252" t="s">
@@ -19608,7 +19611,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="441"/>
+      <c r="A73" s="446"/>
       <c r="B73" s="223" t="s">
         <v>1238</v>
       </c>
@@ -19623,7 +19626,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="441"/>
+      <c r="A74" s="446"/>
       <c r="B74" t="s">
         <v>1240</v>
       </c>
@@ -19641,13 +19644,13 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="441"/>
+      <c r="A75" s="446"/>
       <c r="B75" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="441"/>
+      <c r="A76" s="446"/>
       <c r="B76" t="s">
         <v>1244</v>
       </c>
@@ -20016,19 +20019,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C4:C15"/>
-    <mergeCell ref="D4:D15"/>
-    <mergeCell ref="E4:E15"/>
-    <mergeCell ref="C16:C28"/>
-    <mergeCell ref="E16:E28"/>
-    <mergeCell ref="D16:D28"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="E35:E44"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="E54:E58"/>
-    <mergeCell ref="E61:E65"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="A61:A65"/>
     <mergeCell ref="A67:A69"/>
@@ -20038,6 +20028,19 @@
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A44"/>
     <mergeCell ref="A47:A51"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="E35:E44"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="E54:E58"/>
+    <mergeCell ref="E61:E65"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="D4:D15"/>
+    <mergeCell ref="E4:E15"/>
+    <mergeCell ref="C16:C28"/>
+    <mergeCell ref="E16:E28"/>
+    <mergeCell ref="D16:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20547,20 +20550,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R3" xr:uid="{9C7276AA-1D31-45CB-99BE-1EB8F29BD1DF}"/>
+  <conditionalFormatting sqref="N4:P8">
+    <cfRule type="containsText" dxfId="45" priority="30" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",N4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N2:S3">
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="25" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="26" operator="containsText" text="n/a">
+    <cfRule type="containsText" dxfId="42" priority="26" operator="containsText" text="n/a">
       <formula>NOT(ISERROR(SEARCH("n/a",N2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4:P8">
-    <cfRule type="containsText" dxfId="42" priority="30" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",N4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -23763,15 +23766,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F9864B29171A641B582E76D46C7ACA2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40ac230278d261affbe351c37d5a0641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3fd76951-e4f7-4cc9-8ccb-c4998aa78893" xmlns:ns3="3092193c-6f29-485f-87d2-f467a52e3379" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a5fd78be80f9e1db3d79d02d2c3a784" ns2:_="" ns3:_="">
     <xsd:import namespace="3fd76951-e4f7-4cc9-8ccb-c4998aa78893"/>
@@ -23948,6 +23942,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB274D9-D29B-4016-B1A7-8FC633794465}">
   <ds:schemaRefs>
@@ -23966,14 +23969,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21961765-F20D-4C30-82DC-BD9CF7E6DDAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21444850-BD52-4C83-86F6-A4900F7D7F4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23990,4 +23985,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21961765-F20D-4C30-82DC-BD9CF7E6DDAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- complete review answers implementation
</commit_message>
<xml_diff>
--- a/tests/UnitTests/Rsp.IrasPortal.UnitTests/Data/ValidQuestionSet.xlsx
+++ b/tests/UnitTests/Rsp.IrasPortal.UnitTests/Data/ValidQuestionSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\rsp-iras-portal\tests\UnitTests\Rsp.IrasPortal.UnitTests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C4BAB-E22A-4557-8BCB-36121EC81D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFA1879-6241-4311-8DE0-81233A62D230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26190" windowHeight="11190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="29" r:id="rId1"/>
@@ -39,7 +39,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'App1'!$A$14:$P$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">B!$A$1:$R$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'project record v1'!$A$1:$R$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'project record v1'!$A$1:$S$3</definedName>
     <definedName name="Conformance" localSheetId="0">'[1]App3 Dropdowns'!$D$2:$D$5</definedName>
     <definedName name="Conformance">'App3 Dropdowns'!$D$2:$D$5</definedName>
     <definedName name="DataType" localSheetId="0">'[1]App3 Dropdowns'!$C$2:$C$12</definedName>
@@ -75,7 +75,7 @@
     <author>Joanna Ho</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{B9AF0E57-F6BE-AD4E-AF30-BECDB261DF76}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{B9AF0E57-F6BE-AD4E-AF30-BECDB261DF76}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="1307">
   <si>
     <t>Master Application Questions</t>
   </si>
@@ -6258,6 +6258,9 @@
   </si>
   <si>
     <t>project record v1</t>
+  </si>
+  <si>
+    <t>Short field label</t>
   </si>
 </sst>
 </file>
@@ -7639,7 +7642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="450">
+  <cellXfs count="451">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -8496,6 +8499,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8529,48 +8568,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8583,27 +8586,249 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8634,263 +8859,44 @@
     <xf numFmtId="0" fontId="16" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="66" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9810,7 +9816,7 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
@@ -9856,10 +9862,10 @@
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A2" s="329" t="s">
+      <c r="A2" s="318" t="s">
         <v>1305</v>
       </c>
-      <c r="B2" s="334" t="s">
+      <c r="B2" s="321" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="180" t="s">
@@ -9885,8 +9891,8 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="333"/>
-      <c r="B3" s="335"/>
+      <c r="A3" s="319"/>
+      <c r="B3" s="322"/>
       <c r="C3" s="173" t="s">
         <v>14</v>
       </c>
@@ -9910,8 +9916,8 @@
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="330"/>
-      <c r="B4" s="336"/>
+      <c r="A4" s="320"/>
+      <c r="B4" s="323"/>
       <c r="C4" s="190" t="s">
         <v>16</v>
       </c>
@@ -9932,10 +9938,10 @@
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="329" t="s">
+      <c r="A5" s="318" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="337" t="s">
+      <c r="B5" s="324" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="180" t="s">
@@ -9954,8 +9960,8 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="333"/>
-      <c r="B6" s="338"/>
+      <c r="A6" s="319"/>
+      <c r="B6" s="325"/>
       <c r="C6" s="173" t="s">
         <v>20</v>
       </c>
@@ -9974,8 +9980,8 @@
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="333"/>
-      <c r="B7" s="338"/>
+      <c r="A7" s="319"/>
+      <c r="B7" s="325"/>
       <c r="C7" s="173" t="s">
         <v>21</v>
       </c>
@@ -9996,8 +10002,8 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="333"/>
-      <c r="B8" s="338"/>
+      <c r="A8" s="319"/>
+      <c r="B8" s="325"/>
       <c r="C8" s="173" t="s">
         <v>23</v>
       </c>
@@ -10010,8 +10016,8 @@
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="333"/>
-      <c r="B9" s="338"/>
+      <c r="A9" s="319"/>
+      <c r="B9" s="325"/>
       <c r="C9" s="173" t="s">
         <v>24</v>
       </c>
@@ -10028,8 +10034,8 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="333"/>
-      <c r="B10" s="338"/>
+      <c r="A10" s="319"/>
+      <c r="B10" s="325"/>
       <c r="C10" s="191" t="s">
         <v>25</v>
       </c>
@@ -10043,8 +10049,8 @@
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="333"/>
-      <c r="B11" s="338"/>
+      <c r="A11" s="319"/>
+      <c r="B11" s="325"/>
       <c r="C11" s="191" t="s">
         <v>26</v>
       </c>
@@ -10064,8 +10070,8 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="333"/>
-      <c r="B12" s="338"/>
+      <c r="A12" s="319"/>
+      <c r="B12" s="325"/>
       <c r="C12" s="191" t="s">
         <v>27</v>
       </c>
@@ -10085,8 +10091,8 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="57" x14ac:dyDescent="0.25">
-      <c r="A13" s="333"/>
-      <c r="B13" s="338"/>
+      <c r="A13" s="319"/>
+      <c r="B13" s="325"/>
       <c r="C13" s="191" t="s">
         <v>28</v>
       </c>
@@ -10111,8 +10117,8 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="333"/>
-      <c r="B14" s="338"/>
+      <c r="A14" s="319"/>
+      <c r="B14" s="325"/>
       <c r="C14" s="191" t="s">
         <v>29</v>
       </c>
@@ -10130,8 +10136,8 @@
       <c r="Q14" s="90"/>
     </row>
     <row r="15" spans="1:17" s="79" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="333"/>
-      <c r="B15" s="338"/>
+      <c r="A15" s="319"/>
+      <c r="B15" s="325"/>
       <c r="C15" s="191" t="s">
         <v>30</v>
       </c>
@@ -10157,8 +10163,8 @@
       <c r="Q15" s="90"/>
     </row>
     <row r="16" spans="1:17" s="79" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="330"/>
-      <c r="B16" s="339"/>
+      <c r="A16" s="320"/>
+      <c r="B16" s="326"/>
       <c r="C16" s="193" t="s">
         <v>32</v>
       </c>
@@ -10251,16 +10257,16 @@
       <c r="Q19" s="90"/>
     </row>
     <row r="20" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="340" t="s">
+      <c r="A20" s="327" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="334" t="s">
+      <c r="B20" s="321" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="323" t="s">
+      <c r="D20" s="335" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="238"/>
@@ -10274,12 +10280,12 @@
       <c r="Q20" s="90"/>
     </row>
     <row r="21" spans="1:17" s="79" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="341"/>
-      <c r="B21" s="335"/>
+      <c r="A21" s="328"/>
+      <c r="B21" s="322"/>
       <c r="C21" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="324"/>
+      <c r="D21" s="336"/>
       <c r="F21" s="238"/>
       <c r="G21" s="238"/>
       <c r="H21" s="238"/>
@@ -10291,8 +10297,8 @@
       <c r="Q21" s="90"/>
     </row>
     <row r="22" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="342"/>
-      <c r="B22" s="336"/>
+      <c r="A22" s="329"/>
+      <c r="B22" s="323"/>
       <c r="C22" s="169" t="s">
         <v>49</v>
       </c>
@@ -10323,16 +10329,16 @@
       <c r="Q23" s="90"/>
     </row>
     <row r="24" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="325" t="s">
+      <c r="A24" s="337" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="326" t="s">
+      <c r="B24" s="338" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="323" t="s">
+      <c r="D24" s="335" t="s">
         <v>57</v>
       </c>
       <c r="F24"/>
@@ -10346,12 +10352,12 @@
       <c r="Q24" s="132"/>
     </row>
     <row r="25" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="319"/>
-      <c r="B25" s="327"/>
+      <c r="A25" s="331"/>
+      <c r="B25" s="339"/>
       <c r="C25" s="172" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="328"/>
+      <c r="D25" s="340"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
@@ -10363,10 +10369,10 @@
       <c r="Q25" s="132"/>
     </row>
     <row r="26" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="329" t="s">
+      <c r="A26" s="318" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="331" t="s">
+      <c r="B26" s="341" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="192" t="s">
@@ -10386,8 +10392,8 @@
       <c r="Q26" s="132"/>
     </row>
     <row r="27" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="330"/>
-      <c r="B27" s="332"/>
+      <c r="A27" s="320"/>
+      <c r="B27" s="342"/>
       <c r="C27" s="190" t="s">
         <v>63</v>
       </c>
@@ -10445,10 +10451,10 @@
       <c r="Q29" s="132"/>
     </row>
     <row r="30" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="318" t="s">
+      <c r="A30" s="330" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="321" t="s">
+      <c r="B30" s="333" t="s">
         <v>72</v>
       </c>
       <c r="C30" s="174" t="s">
@@ -10468,8 +10474,8 @@
       <c r="Q30" s="132"/>
     </row>
     <row r="31" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="319"/>
-      <c r="B31" s="321"/>
+      <c r="A31" s="331"/>
+      <c r="B31" s="333"/>
       <c r="C31" s="191" t="s">
         <v>75</v>
       </c>
@@ -10487,8 +10493,8 @@
       <c r="Q31" s="132"/>
     </row>
     <row r="32" spans="1:17" s="79" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="319"/>
-      <c r="B32" s="321"/>
+      <c r="A32" s="331"/>
+      <c r="B32" s="333"/>
       <c r="C32" s="191" t="s">
         <v>77</v>
       </c>
@@ -10506,8 +10512,8 @@
       <c r="Q32" s="132"/>
     </row>
     <row r="33" spans="1:17" s="79" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="320"/>
-      <c r="B33" s="322"/>
+      <c r="A33" s="332"/>
+      <c r="B33" s="334"/>
       <c r="C33" s="175"/>
       <c r="D33" s="161"/>
       <c r="F33" s="92"/>
@@ -10736,12 +10742,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A16"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="D20:D21"/>
@@ -10750,6 +10750,12 @@
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" location="A!E5" display="Project details" xr:uid="{4428746E-4300-4BD2-985A-60358BBE6AB0}"/>
@@ -13690,10 +13696,10 @@
       <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="404" t="s">
+      <c r="B4" s="376" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="405"/>
+      <c r="C4" s="377"/>
       <c r="D4" s="63" t="s">
         <v>242</v>
       </c>
@@ -13736,8 +13742,8 @@
       <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="1:17" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="406"/>
-      <c r="C5" s="407"/>
+      <c r="B5" s="378"/>
+      <c r="C5" s="379"/>
       <c r="D5" s="64" t="s">
         <v>243</v>
       </c>
@@ -13782,7 +13788,7 @@
       <c r="B6" s="207">
         <v>1</v>
       </c>
-      <c r="C6" s="411" t="s">
+      <c r="C6" s="383" t="s">
         <v>255</v>
       </c>
       <c r="D6" s="43" t="s">
@@ -13829,7 +13835,7 @@
       <c r="B7" s="42">
         <v>2</v>
       </c>
-      <c r="C7" s="411"/>
+      <c r="C7" s="383"/>
       <c r="D7" s="46" t="s">
         <v>258</v>
       </c>
@@ -13874,7 +13880,7 @@
       <c r="B8" s="42">
         <v>3</v>
       </c>
-      <c r="C8" s="411"/>
+      <c r="C8" s="383"/>
       <c r="D8" s="46" t="s">
         <v>259</v>
       </c>
@@ -13907,7 +13913,7 @@
       <c r="B9" s="42">
         <v>4</v>
       </c>
-      <c r="C9" s="411"/>
+      <c r="C9" s="383"/>
       <c r="D9" s="46" t="s">
         <v>260</v>
       </c>
@@ -13935,7 +13941,7 @@
       <c r="B10" s="199">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C10" s="411"/>
+      <c r="C10" s="383"/>
       <c r="D10" s="198" t="s">
         <v>261</v>
       </c>
@@ -13978,7 +13984,7 @@
       <c r="B11" s="42">
         <v>5</v>
       </c>
-      <c r="C11" s="411"/>
+      <c r="C11" s="383"/>
       <c r="D11" s="46" t="s">
         <v>262</v>
       </c>
@@ -14021,7 +14027,7 @@
       <c r="B12" s="42">
         <v>6</v>
       </c>
-      <c r="C12" s="411"/>
+      <c r="C12" s="383"/>
       <c r="D12" s="46" t="s">
         <v>263</v>
       </c>
@@ -14063,7 +14069,7 @@
       <c r="B13" s="42">
         <v>7</v>
       </c>
-      <c r="C13" s="412"/>
+      <c r="C13" s="384"/>
       <c r="D13" s="48" t="s">
         <v>264</v>
       </c>
@@ -14104,24 +14110,24 @@
     </row>
     <row r="15" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51"/>
-      <c r="C15" s="401" t="s">
+      <c r="C15" s="373" t="s">
         <v>265</v>
       </c>
-      <c r="D15" s="402"/>
-      <c r="E15" s="413" t="s">
+      <c r="D15" s="374"/>
+      <c r="E15" s="385" t="s">
         <v>266</v>
       </c>
-      <c r="F15" s="414"/>
-      <c r="G15" s="414"/>
-      <c r="H15" s="414"/>
-      <c r="I15" s="414"/>
-      <c r="J15" s="414"/>
-      <c r="K15" s="414"/>
-      <c r="L15" s="414"/>
-      <c r="M15" s="414"/>
-      <c r="N15" s="414"/>
-      <c r="O15" s="414"/>
-      <c r="P15" s="414"/>
+      <c r="F15" s="386"/>
+      <c r="G15" s="386"/>
+      <c r="H15" s="386"/>
+      <c r="I15" s="386"/>
+      <c r="J15" s="386"/>
+      <c r="K15" s="386"/>
+      <c r="L15" s="386"/>
+      <c r="M15" s="386"/>
+      <c r="N15" s="386"/>
+      <c r="O15" s="386"/>
+      <c r="P15" s="386"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
@@ -14130,37 +14136,37 @@
       <c r="D16" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="409" t="s">
+      <c r="E16" s="381" t="s">
         <v>268</v>
       </c>
-      <c r="F16" s="409"/>
-      <c r="G16" s="409"/>
-      <c r="H16" s="409"/>
-      <c r="I16" s="409"/>
-      <c r="J16" s="409"/>
-      <c r="K16" s="409"/>
-      <c r="L16" s="409"/>
-      <c r="M16" s="409"/>
-      <c r="N16" s="409"/>
-      <c r="O16" s="409"/>
-      <c r="P16" s="409"/>
+      <c r="F16" s="381"/>
+      <c r="G16" s="381"/>
+      <c r="H16" s="381"/>
+      <c r="I16" s="381"/>
+      <c r="J16" s="381"/>
+      <c r="K16" s="381"/>
+      <c r="L16" s="381"/>
+      <c r="M16" s="381"/>
+      <c r="N16" s="381"/>
+      <c r="O16" s="381"/>
+      <c r="P16" s="381"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="403" t="s">
+      <c r="D17" s="375" t="s">
         <v>269</v>
       </c>
-      <c r="E17" s="403"/>
-      <c r="F17" s="403"/>
-      <c r="G17" s="403"/>
-      <c r="H17" s="403"/>
-      <c r="I17" s="403"/>
-      <c r="J17" s="403"/>
-      <c r="K17" s="403"/>
-      <c r="L17" s="403"/>
-      <c r="M17" s="403"/>
-      <c r="N17" s="403"/>
-      <c r="O17" s="403"/>
-      <c r="P17" s="403"/>
+      <c r="E17" s="375"/>
+      <c r="F17" s="375"/>
+      <c r="G17" s="375"/>
+      <c r="H17" s="375"/>
+      <c r="I17" s="375"/>
+      <c r="J17" s="375"/>
+      <c r="K17" s="375"/>
+      <c r="L17" s="375"/>
+      <c r="M17" s="375"/>
+      <c r="N17" s="375"/>
+      <c r="O17" s="375"/>
+      <c r="P17" s="375"/>
     </row>
     <row r="18" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="42">
@@ -14169,20 +14175,20 @@
       <c r="D18" s="68" t="s">
         <v>270</v>
       </c>
-      <c r="E18" s="408" t="s">
+      <c r="E18" s="380" t="s">
         <v>271</v>
       </c>
-      <c r="F18" s="409"/>
-      <c r="G18" s="409"/>
-      <c r="H18" s="409"/>
-      <c r="I18" s="409"/>
-      <c r="J18" s="409"/>
-      <c r="K18" s="409"/>
-      <c r="L18" s="409"/>
-      <c r="M18" s="409"/>
-      <c r="N18" s="409"/>
-      <c r="O18" s="409"/>
-      <c r="P18" s="409"/>
+      <c r="F18" s="381"/>
+      <c r="G18" s="381"/>
+      <c r="H18" s="381"/>
+      <c r="I18" s="381"/>
+      <c r="J18" s="381"/>
+      <c r="K18" s="381"/>
+      <c r="L18" s="381"/>
+      <c r="M18" s="381"/>
+      <c r="N18" s="381"/>
+      <c r="O18" s="381"/>
+      <c r="P18" s="381"/>
     </row>
     <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="42">
@@ -14191,20 +14197,20 @@
       <c r="D19" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="E19" s="399" t="s">
+      <c r="E19" s="371" t="s">
         <v>273</v>
       </c>
-      <c r="F19" s="400"/>
-      <c r="G19" s="400"/>
-      <c r="H19" s="400"/>
-      <c r="I19" s="400"/>
-      <c r="J19" s="400"/>
-      <c r="K19" s="400"/>
-      <c r="L19" s="400"/>
-      <c r="M19" s="400"/>
-      <c r="N19" s="400"/>
-      <c r="O19" s="400"/>
-      <c r="P19" s="400"/>
+      <c r="F19" s="372"/>
+      <c r="G19" s="372"/>
+      <c r="H19" s="372"/>
+      <c r="I19" s="372"/>
+      <c r="J19" s="372"/>
+      <c r="K19" s="372"/>
+      <c r="L19" s="372"/>
+      <c r="M19" s="372"/>
+      <c r="N19" s="372"/>
+      <c r="O19" s="372"/>
+      <c r="P19" s="372"/>
     </row>
     <row r="20" spans="1:16" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="42">
@@ -14213,20 +14219,20 @@
       <c r="D20" s="53" t="s">
         <v>274</v>
       </c>
-      <c r="E20" s="399" t="s">
+      <c r="E20" s="371" t="s">
         <v>275</v>
       </c>
-      <c r="F20" s="400"/>
-      <c r="G20" s="400"/>
-      <c r="H20" s="400"/>
-      <c r="I20" s="400"/>
-      <c r="J20" s="400"/>
-      <c r="K20" s="400"/>
-      <c r="L20" s="400"/>
-      <c r="M20" s="400"/>
-      <c r="N20" s="400"/>
-      <c r="O20" s="400"/>
-      <c r="P20" s="400"/>
+      <c r="F20" s="372"/>
+      <c r="G20" s="372"/>
+      <c r="H20" s="372"/>
+      <c r="I20" s="372"/>
+      <c r="J20" s="372"/>
+      <c r="K20" s="372"/>
+      <c r="L20" s="372"/>
+      <c r="M20" s="372"/>
+      <c r="N20" s="372"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="372"/>
     </row>
     <row r="21" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="42">
@@ -14235,20 +14241,20 @@
       <c r="D21" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="E21" s="410" t="s">
+      <c r="E21" s="382" t="s">
         <v>277</v>
       </c>
-      <c r="F21" s="410"/>
-      <c r="G21" s="410"/>
-      <c r="H21" s="410"/>
-      <c r="I21" s="410"/>
-      <c r="J21" s="410"/>
-      <c r="K21" s="410"/>
-      <c r="L21" s="410"/>
-      <c r="M21" s="410"/>
-      <c r="N21" s="410"/>
-      <c r="O21" s="410"/>
-      <c r="P21" s="410"/>
+      <c r="F21" s="382"/>
+      <c r="G21" s="382"/>
+      <c r="H21" s="382"/>
+      <c r="I21" s="382"/>
+      <c r="J21" s="382"/>
+      <c r="K21" s="382"/>
+      <c r="L21" s="382"/>
+      <c r="M21" s="382"/>
+      <c r="N21" s="382"/>
+      <c r="O21" s="382"/>
+      <c r="P21" s="382"/>
     </row>
     <row r="22" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="199">
@@ -14257,20 +14263,20 @@
       <c r="D22" s="208" t="s">
         <v>278</v>
       </c>
-      <c r="E22" s="415" t="s">
+      <c r="E22" s="387" t="s">
         <v>279</v>
       </c>
-      <c r="F22" s="416"/>
-      <c r="G22" s="416"/>
-      <c r="H22" s="416"/>
-      <c r="I22" s="416"/>
-      <c r="J22" s="416"/>
-      <c r="K22" s="416"/>
-      <c r="L22" s="416"/>
-      <c r="M22" s="416"/>
-      <c r="N22" s="416"/>
-      <c r="O22" s="416"/>
-      <c r="P22" s="417"/>
+      <c r="F22" s="388"/>
+      <c r="G22" s="388"/>
+      <c r="H22" s="388"/>
+      <c r="I22" s="388"/>
+      <c r="J22" s="388"/>
+      <c r="K22" s="388"/>
+      <c r="L22" s="388"/>
+      <c r="M22" s="388"/>
+      <c r="N22" s="388"/>
+      <c r="O22" s="388"/>
+      <c r="P22" s="389"/>
     </row>
     <row r="23" spans="1:16" ht="152.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="42">
@@ -14279,20 +14285,20 @@
       <c r="D23" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="E23" s="399" t="s">
+      <c r="E23" s="371" t="s">
         <v>281</v>
       </c>
-      <c r="F23" s="400"/>
-      <c r="G23" s="400"/>
-      <c r="H23" s="400"/>
-      <c r="I23" s="400"/>
-      <c r="J23" s="400"/>
-      <c r="K23" s="400"/>
-      <c r="L23" s="400"/>
-      <c r="M23" s="400"/>
-      <c r="N23" s="400"/>
-      <c r="O23" s="400"/>
-      <c r="P23" s="400"/>
+      <c r="F23" s="372"/>
+      <c r="G23" s="372"/>
+      <c r="H23" s="372"/>
+      <c r="I23" s="372"/>
+      <c r="J23" s="372"/>
+      <c r="K23" s="372"/>
+      <c r="L23" s="372"/>
+      <c r="M23" s="372"/>
+      <c r="N23" s="372"/>
+      <c r="O23" s="372"/>
+      <c r="P23" s="372"/>
     </row>
     <row r="24" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="42">
@@ -14301,20 +14307,20 @@
       <c r="D24" s="53" t="s">
         <v>282</v>
       </c>
-      <c r="E24" s="399" t="s">
+      <c r="E24" s="371" t="s">
         <v>283</v>
       </c>
-      <c r="F24" s="400"/>
-      <c r="G24" s="400"/>
-      <c r="H24" s="400"/>
-      <c r="I24" s="400"/>
-      <c r="J24" s="400"/>
-      <c r="K24" s="400"/>
-      <c r="L24" s="400"/>
-      <c r="M24" s="400"/>
-      <c r="N24" s="400"/>
-      <c r="O24" s="400"/>
-      <c r="P24" s="400"/>
+      <c r="F24" s="372"/>
+      <c r="G24" s="372"/>
+      <c r="H24" s="372"/>
+      <c r="I24" s="372"/>
+      <c r="J24" s="372"/>
+      <c r="K24" s="372"/>
+      <c r="L24" s="372"/>
+      <c r="M24" s="372"/>
+      <c r="N24" s="372"/>
+      <c r="O24" s="372"/>
+      <c r="P24" s="372"/>
     </row>
     <row r="25" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="42">
@@ -14323,20 +14329,20 @@
       <c r="D25" s="53" t="s">
         <v>284</v>
       </c>
-      <c r="E25" s="399" t="s">
+      <c r="E25" s="371" t="s">
         <v>285</v>
       </c>
-      <c r="F25" s="400"/>
-      <c r="G25" s="400"/>
-      <c r="H25" s="400"/>
-      <c r="I25" s="400"/>
-      <c r="J25" s="400"/>
-      <c r="K25" s="400"/>
-      <c r="L25" s="400"/>
-      <c r="M25" s="400"/>
-      <c r="N25" s="400"/>
-      <c r="O25" s="400"/>
-      <c r="P25" s="400"/>
+      <c r="F25" s="372"/>
+      <c r="G25" s="372"/>
+      <c r="H25" s="372"/>
+      <c r="I25" s="372"/>
+      <c r="J25" s="372"/>
+      <c r="K25" s="372"/>
+      <c r="L25" s="372"/>
+      <c r="M25" s="372"/>
+      <c r="N25" s="372"/>
+      <c r="O25" s="372"/>
+      <c r="P25" s="372"/>
     </row>
     <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="78" t="s">
@@ -14352,184 +14358,184 @@
       <c r="E30" s="81"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="398" t="s">
+      <c r="B31" s="390" t="s">
         <v>287</v>
       </c>
-      <c r="C31" s="398"/>
+      <c r="C31" s="390"/>
       <c r="D31" s="82" t="s">
         <v>288</v>
       </c>
-      <c r="E31" s="398" t="s">
+      <c r="E31" s="390" t="s">
         <v>289</v>
       </c>
-      <c r="F31" s="398"/>
-      <c r="G31" s="398"/>
-      <c r="H31" s="398"/>
-      <c r="I31" s="398"/>
-      <c r="J31" s="398"/>
-      <c r="K31" s="398"/>
+      <c r="F31" s="390"/>
+      <c r="G31" s="390"/>
+      <c r="H31" s="390"/>
+      <c r="I31" s="390"/>
+      <c r="J31" s="390"/>
+      <c r="K31" s="390"/>
     </row>
     <row r="32" spans="1:16" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="388" t="s">
+      <c r="B32" s="392" t="s">
         <v>290</v>
       </c>
-      <c r="C32" s="388"/>
+      <c r="C32" s="392"/>
       <c r="D32" s="84" t="s">
         <v>291</v>
       </c>
-      <c r="E32" s="389" t="s">
+      <c r="E32" s="391" t="s">
         <v>292</v>
       </c>
-      <c r="F32" s="389"/>
-      <c r="G32" s="389"/>
-      <c r="H32" s="389"/>
-      <c r="I32" s="389"/>
-      <c r="J32" s="389"/>
-      <c r="K32" s="389"/>
+      <c r="F32" s="391"/>
+      <c r="G32" s="391"/>
+      <c r="H32" s="391"/>
+      <c r="I32" s="391"/>
+      <c r="J32" s="391"/>
+      <c r="K32" s="391"/>
     </row>
     <row r="33" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="388" t="s">
+      <c r="B33" s="392" t="s">
         <v>293</v>
       </c>
-      <c r="C33" s="388"/>
+      <c r="C33" s="392"/>
       <c r="D33" s="85" t="s">
         <v>294</v>
       </c>
-      <c r="E33" s="389" t="s">
+      <c r="E33" s="391" t="s">
         <v>295</v>
       </c>
-      <c r="F33" s="389"/>
-      <c r="G33" s="389"/>
-      <c r="H33" s="389"/>
-      <c r="I33" s="389"/>
-      <c r="J33" s="389"/>
-      <c r="K33" s="389"/>
+      <c r="F33" s="391"/>
+      <c r="G33" s="391"/>
+      <c r="H33" s="391"/>
+      <c r="I33" s="391"/>
+      <c r="J33" s="391"/>
+      <c r="K33" s="391"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="388" t="s">
+      <c r="B34" s="392" t="s">
         <v>296</v>
       </c>
-      <c r="C34" s="388"/>
+      <c r="C34" s="392"/>
       <c r="D34" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="E34" s="391" t="s">
+      <c r="E34" s="393" t="s">
         <v>298</v>
       </c>
-      <c r="F34" s="391"/>
-      <c r="G34" s="391"/>
-      <c r="H34" s="391"/>
-      <c r="I34" s="391"/>
-      <c r="J34" s="391"/>
-      <c r="K34" s="391"/>
+      <c r="F34" s="393"/>
+      <c r="G34" s="393"/>
+      <c r="H34" s="393"/>
+      <c r="I34" s="393"/>
+      <c r="J34" s="393"/>
+      <c r="K34" s="393"/>
     </row>
     <row r="35" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="390" t="s">
+      <c r="B35" s="394" t="s">
         <v>299</v>
       </c>
-      <c r="C35" s="390"/>
+      <c r="C35" s="394"/>
       <c r="D35" s="86" t="s">
         <v>300</v>
       </c>
-      <c r="E35" s="389" t="s">
+      <c r="E35" s="391" t="s">
         <v>301</v>
       </c>
-      <c r="F35" s="389"/>
-      <c r="G35" s="389"/>
-      <c r="H35" s="389"/>
-      <c r="I35" s="389"/>
-      <c r="J35" s="389"/>
-      <c r="K35" s="389"/>
+      <c r="F35" s="391"/>
+      <c r="G35" s="391"/>
+      <c r="H35" s="391"/>
+      <c r="I35" s="391"/>
+      <c r="J35" s="391"/>
+      <c r="K35" s="391"/>
     </row>
     <row r="36" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="388" t="s">
+      <c r="B36" s="392" t="s">
         <v>302</v>
       </c>
-      <c r="C36" s="388"/>
+      <c r="C36" s="392"/>
       <c r="D36" s="83" t="s">
         <v>303</v>
       </c>
-      <c r="E36" s="391" t="s">
+      <c r="E36" s="393" t="s">
         <v>304</v>
       </c>
-      <c r="F36" s="397"/>
-      <c r="G36" s="397"/>
-      <c r="H36" s="397"/>
-      <c r="I36" s="397"/>
-      <c r="J36" s="397"/>
-      <c r="K36" s="397"/>
+      <c r="F36" s="395"/>
+      <c r="G36" s="395"/>
+      <c r="H36" s="395"/>
+      <c r="I36" s="395"/>
+      <c r="J36" s="395"/>
+      <c r="K36" s="395"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="388" t="s">
+      <c r="B37" s="392" t="s">
         <v>305</v>
       </c>
-      <c r="C37" s="388"/>
+      <c r="C37" s="392"/>
       <c r="D37" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="E37" s="389" t="s">
+      <c r="E37" s="391" t="s">
         <v>307</v>
       </c>
-      <c r="F37" s="389"/>
-      <c r="G37" s="389"/>
-      <c r="H37" s="389"/>
-      <c r="I37" s="389"/>
-      <c r="J37" s="389"/>
-      <c r="K37" s="389"/>
+      <c r="F37" s="391"/>
+      <c r="G37" s="391"/>
+      <c r="H37" s="391"/>
+      <c r="I37" s="391"/>
+      <c r="J37" s="391"/>
+      <c r="K37" s="391"/>
     </row>
     <row r="38" spans="1:11" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="392" t="s">
+      <c r="B38" s="396" t="s">
         <v>308</v>
       </c>
-      <c r="C38" s="393"/>
+      <c r="C38" s="397"/>
       <c r="D38" s="86" t="s">
         <v>309</v>
       </c>
-      <c r="E38" s="394" t="s">
+      <c r="E38" s="398" t="s">
         <v>310</v>
       </c>
-      <c r="F38" s="395"/>
-      <c r="G38" s="395"/>
-      <c r="H38" s="395"/>
-      <c r="I38" s="395"/>
-      <c r="J38" s="395"/>
-      <c r="K38" s="396"/>
+      <c r="F38" s="399"/>
+      <c r="G38" s="399"/>
+      <c r="H38" s="399"/>
+      <c r="I38" s="399"/>
+      <c r="J38" s="399"/>
+      <c r="K38" s="400"/>
     </row>
     <row r="39" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="390" t="s">
+      <c r="B39" s="394" t="s">
         <v>311</v>
       </c>
-      <c r="C39" s="390"/>
+      <c r="C39" s="394"/>
       <c r="D39" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="E39" s="391" t="s">
+      <c r="E39" s="393" t="s">
         <v>313</v>
       </c>
-      <c r="F39" s="391"/>
-      <c r="G39" s="391"/>
-      <c r="H39" s="391"/>
-      <c r="I39" s="391"/>
-      <c r="J39" s="391"/>
-      <c r="K39" s="391"/>
+      <c r="F39" s="393"/>
+      <c r="G39" s="393"/>
+      <c r="H39" s="393"/>
+      <c r="I39" s="393"/>
+      <c r="J39" s="393"/>
+      <c r="K39" s="393"/>
     </row>
     <row r="40" spans="1:11" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="388" t="s">
+      <c r="B40" s="392" t="s">
         <v>314</v>
       </c>
-      <c r="C40" s="388"/>
+      <c r="C40" s="392"/>
       <c r="D40" s="84" t="s">
         <v>315</v>
       </c>
-      <c r="E40" s="391" t="s">
+      <c r="E40" s="393" t="s">
         <v>316</v>
       </c>
-      <c r="F40" s="391"/>
-      <c r="G40" s="391"/>
-      <c r="H40" s="391"/>
-      <c r="I40" s="391"/>
-      <c r="J40" s="391"/>
-      <c r="K40" s="391"/>
+      <c r="F40" s="393"/>
+      <c r="G40" s="393"/>
+      <c r="H40" s="393"/>
+      <c r="I40" s="393"/>
+      <c r="J40" s="393"/>
+      <c r="K40" s="393"/>
     </row>
     <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="78" t="s">
@@ -14547,11 +14553,11 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A47" s="380" t="s">
+      <c r="A47" s="414" t="s">
         <v>319</v>
       </c>
-      <c r="B47" s="378"/>
-      <c r="C47" s="378"/>
+      <c r="B47" s="412"/>
+      <c r="C47" s="412"/>
       <c r="D47" s="141" t="s">
         <v>320</v>
       </c>
@@ -14567,18 +14573,18 @@
       <c r="H47" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="I47" s="377" t="s">
+      <c r="I47" s="411" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="378"/>
-      <c r="K47" s="379"/>
+      <c r="J47" s="412"/>
+      <c r="K47" s="413"/>
     </row>
     <row r="48" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="373" t="s">
+      <c r="A48" s="403" t="s">
         <v>323</v>
       </c>
-      <c r="B48" s="366"/>
-      <c r="C48" s="366"/>
+      <c r="B48" s="404"/>
+      <c r="C48" s="404"/>
       <c r="D48" s="91" t="s">
         <v>324</v>
       </c>
@@ -14594,37 +14600,37 @@
       <c r="H48" s="87" t="s">
         <v>326</v>
       </c>
-      <c r="I48" s="381" t="s">
+      <c r="I48" s="415" t="s">
         <v>327</v>
       </c>
-      <c r="J48" s="381"/>
-      <c r="K48" s="382"/>
+      <c r="J48" s="415"/>
+      <c r="K48" s="416"/>
     </row>
     <row r="49" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="373" t="s">
+      <c r="A49" s="403" t="s">
         <v>328</v>
       </c>
-      <c r="B49" s="366"/>
-      <c r="C49" s="366"/>
+      <c r="B49" s="404"/>
+      <c r="C49" s="404"/>
       <c r="D49" s="91" t="s">
         <v>329</v>
       </c>
-      <c r="E49" s="428" t="s">
+      <c r="E49" s="357" t="s">
         <v>330</v>
       </c>
-      <c r="F49" s="428"/>
-      <c r="G49" s="428"/>
-      <c r="H49" s="428"/>
-      <c r="I49" s="428"/>
-      <c r="J49" s="428"/>
-      <c r="K49" s="429"/>
+      <c r="F49" s="357"/>
+      <c r="G49" s="357"/>
+      <c r="H49" s="357"/>
+      <c r="I49" s="357"/>
+      <c r="J49" s="357"/>
+      <c r="K49" s="358"/>
     </row>
     <row r="50" spans="1:11" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="373" t="s">
+      <c r="A50" s="403" t="s">
         <v>331</v>
       </c>
-      <c r="B50" s="366"/>
-      <c r="C50" s="366"/>
+      <c r="B50" s="404"/>
+      <c r="C50" s="404"/>
       <c r="D50" s="126" t="s">
         <v>332</v>
       </c>
@@ -14640,16 +14646,16 @@
       <c r="H50" s="98" t="s">
         <v>334</v>
       </c>
-      <c r="I50" s="381" t="s">
+      <c r="I50" s="415" t="s">
         <v>335</v>
       </c>
-      <c r="J50" s="381"/>
-      <c r="K50" s="382"/>
+      <c r="J50" s="415"/>
+      <c r="K50" s="416"/>
     </row>
     <row r="51" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="373"/>
-      <c r="B51" s="366"/>
-      <c r="C51" s="366"/>
+      <c r="A51" s="403"/>
+      <c r="B51" s="404"/>
+      <c r="C51" s="404"/>
       <c r="D51" s="127" t="s">
         <v>336</v>
       </c>
@@ -14665,19 +14671,19 @@
       <c r="H51" s="87" t="s">
         <v>338</v>
       </c>
-      <c r="I51" s="383" t="s">
+      <c r="I51" s="417" t="s">
         <v>339</v>
       </c>
-      <c r="J51" s="383"/>
-      <c r="K51" s="384"/>
+      <c r="J51" s="417"/>
+      <c r="K51" s="418"/>
     </row>
     <row r="52" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="373" t="s">
+      <c r="A52" s="403" t="s">
         <v>340</v>
       </c>
-      <c r="B52" s="366"/>
-      <c r="C52" s="366"/>
-      <c r="D52" s="376" t="s">
+      <c r="B52" s="404"/>
+      <c r="C52" s="404"/>
+      <c r="D52" s="410" t="s">
         <v>341</v>
       </c>
       <c r="E52" s="137" t="s">
@@ -14692,17 +14698,17 @@
       <c r="H52" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I52" s="368" t="s">
+      <c r="I52" s="419" t="s">
         <v>343</v>
       </c>
-      <c r="J52" s="368"/>
-      <c r="K52" s="369"/>
+      <c r="J52" s="419"/>
+      <c r="K52" s="420"/>
     </row>
     <row r="53" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="374"/>
-      <c r="B53" s="375"/>
-      <c r="C53" s="375"/>
-      <c r="D53" s="376"/>
+      <c r="A53" s="405"/>
+      <c r="B53" s="406"/>
+      <c r="C53" s="406"/>
+      <c r="D53" s="410"/>
       <c r="E53" s="128" t="s">
         <v>344</v>
       </c>
@@ -14715,18 +14721,18 @@
       <c r="H53" s="101">
         <v>1</v>
       </c>
-      <c r="I53" s="364" t="s">
+      <c r="I53" s="369" t="s">
         <v>345</v>
       </c>
-      <c r="J53" s="364"/>
-      <c r="K53" s="365"/>
+      <c r="J53" s="369"/>
+      <c r="K53" s="370"/>
     </row>
     <row r="54" spans="1:11" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="367" t="s">
+      <c r="A54" s="401" t="s">
         <v>346</v>
       </c>
-      <c r="B54" s="347"/>
-      <c r="C54" s="347"/>
+      <c r="B54" s="402"/>
+      <c r="C54" s="402"/>
       <c r="D54" s="122" t="s">
         <v>347</v>
       </c>
@@ -14742,18 +14748,18 @@
       <c r="H54" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I54" s="368" t="s">
+      <c r="I54" s="419" t="s">
         <v>349</v>
       </c>
-      <c r="J54" s="368"/>
-      <c r="K54" s="369"/>
+      <c r="J54" s="419"/>
+      <c r="K54" s="420"/>
     </row>
     <row r="55" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="367" t="s">
+      <c r="A55" s="401" t="s">
         <v>350</v>
       </c>
-      <c r="B55" s="347"/>
-      <c r="C55" s="347"/>
+      <c r="B55" s="402"/>
+      <c r="C55" s="402"/>
       <c r="D55" s="122" t="s">
         <v>351</v>
       </c>
@@ -14769,18 +14775,18 @@
       <c r="H55" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="I55" s="368" t="s">
+      <c r="I55" s="419" t="s">
         <v>353</v>
       </c>
-      <c r="J55" s="368"/>
-      <c r="K55" s="369"/>
+      <c r="J55" s="419"/>
+      <c r="K55" s="420"/>
     </row>
     <row r="56" spans="1:11" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="373" t="s">
+      <c r="A56" s="403" t="s">
         <v>354</v>
       </c>
-      <c r="B56" s="366"/>
-      <c r="C56" s="366"/>
+      <c r="B56" s="404"/>
+      <c r="C56" s="404"/>
       <c r="D56" s="122" t="s">
         <v>355</v>
       </c>
@@ -14796,18 +14802,18 @@
       <c r="H56" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="I56" s="370" t="s">
+      <c r="I56" s="421" t="s">
         <v>358</v>
       </c>
-      <c r="J56" s="371"/>
-      <c r="K56" s="372"/>
+      <c r="J56" s="422"/>
+      <c r="K56" s="423"/>
     </row>
     <row r="57" spans="1:11" ht="261" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="374" t="s">
+      <c r="A57" s="405" t="s">
         <v>359</v>
       </c>
-      <c r="B57" s="375"/>
-      <c r="C57" s="375"/>
+      <c r="B57" s="406"/>
+      <c r="C57" s="406"/>
       <c r="D57" s="108" t="s">
         <v>360</v>
       </c>
@@ -14823,18 +14829,18 @@
       <c r="H57" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="I57" s="370" t="s">
+      <c r="I57" s="421" t="s">
         <v>363</v>
       </c>
-      <c r="J57" s="371"/>
-      <c r="K57" s="372"/>
+      <c r="J57" s="422"/>
+      <c r="K57" s="423"/>
     </row>
     <row r="58" spans="1:11" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="367" t="s">
+      <c r="A58" s="401" t="s">
         <v>364</v>
       </c>
-      <c r="B58" s="347"/>
-      <c r="C58" s="347"/>
+      <c r="B58" s="402"/>
+      <c r="C58" s="402"/>
       <c r="D58" s="91" t="s">
         <v>365</v>
       </c>
@@ -14850,18 +14856,18 @@
       <c r="H58" s="33">
         <v>1</v>
       </c>
-      <c r="I58" s="352" t="s">
+      <c r="I58" s="424" t="s">
         <v>366</v>
       </c>
-      <c r="J58" s="352"/>
-      <c r="K58" s="353"/>
+      <c r="J58" s="424"/>
+      <c r="K58" s="425"/>
     </row>
     <row r="59" spans="1:11" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="367" t="s">
+      <c r="A59" s="401" t="s">
         <v>367</v>
       </c>
-      <c r="B59" s="347"/>
-      <c r="C59" s="347"/>
+      <c r="B59" s="402"/>
+      <c r="C59" s="402"/>
       <c r="D59" s="122" t="s">
         <v>368</v>
       </c>
@@ -14877,18 +14883,18 @@
       <c r="H59" s="34">
         <v>3</v>
       </c>
-      <c r="I59" s="352" t="s">
+      <c r="I59" s="424" t="s">
         <v>133</v>
       </c>
-      <c r="J59" s="352"/>
-      <c r="K59" s="353"/>
+      <c r="J59" s="424"/>
+      <c r="K59" s="425"/>
     </row>
     <row r="60" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="373" t="s">
+      <c r="A60" s="403" t="s">
         <v>369</v>
       </c>
-      <c r="B60" s="366"/>
-      <c r="C60" s="366"/>
+      <c r="B60" s="404"/>
+      <c r="C60" s="404"/>
       <c r="D60" s="122" t="s">
         <v>370</v>
       </c>
@@ -14904,18 +14910,18 @@
       <c r="H60" s="89" t="s">
         <v>191</v>
       </c>
-      <c r="I60" s="350" t="s">
+      <c r="I60" s="359" t="s">
         <v>146</v>
       </c>
-      <c r="J60" s="350"/>
-      <c r="K60" s="351"/>
+      <c r="J60" s="359"/>
+      <c r="K60" s="360"/>
     </row>
     <row r="61" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A61" s="373" t="s">
+      <c r="A61" s="403" t="s">
         <v>371</v>
       </c>
-      <c r="B61" s="366"/>
-      <c r="C61" s="366"/>
+      <c r="B61" s="404"/>
+      <c r="C61" s="404"/>
       <c r="D61" s="122" t="s">
         <v>372</v>
       </c>
@@ -14931,60 +14937,60 @@
       <c r="H61" s="87">
         <v>1</v>
       </c>
-      <c r="I61" s="364" t="s">
+      <c r="I61" s="369" t="s">
         <v>374</v>
       </c>
-      <c r="J61" s="364"/>
-      <c r="K61" s="365"/>
+      <c r="J61" s="369"/>
+      <c r="K61" s="370"/>
     </row>
     <row r="62" spans="1:11" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="354" t="s">
+      <c r="A62" s="428" t="s">
         <v>375</v>
       </c>
-      <c r="B62" s="355"/>
-      <c r="C62" s="356"/>
+      <c r="B62" s="429"/>
+      <c r="C62" s="430"/>
       <c r="D62" s="121" t="s">
         <v>376</v>
       </c>
-      <c r="E62" s="433" t="s">
+      <c r="E62" s="364" t="s">
         <v>377</v>
       </c>
-      <c r="F62" s="434" t="s">
+      <c r="F62" s="365" t="s">
         <v>12</v>
       </c>
-      <c r="G62" s="434" t="s">
+      <c r="G62" s="365" t="s">
         <v>24</v>
       </c>
-      <c r="H62" s="435">
+      <c r="H62" s="366">
         <v>1</v>
       </c>
-      <c r="I62" s="350" t="s">
+      <c r="I62" s="359" t="s">
         <v>378</v>
       </c>
-      <c r="J62" s="350"/>
-      <c r="K62" s="351"/>
+      <c r="J62" s="359"/>
+      <c r="K62" s="360"/>
     </row>
     <row r="63" spans="1:11" ht="180.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="357"/>
-      <c r="B63" s="358"/>
-      <c r="C63" s="359"/>
+      <c r="A63" s="431"/>
+      <c r="B63" s="432"/>
+      <c r="C63" s="433"/>
       <c r="D63" s="125" t="s">
         <v>379</v>
       </c>
-      <c r="E63" s="433"/>
-      <c r="F63" s="434"/>
-      <c r="G63" s="434"/>
-      <c r="H63" s="435"/>
-      <c r="I63" s="436"/>
-      <c r="J63" s="436"/>
-      <c r="K63" s="437"/>
+      <c r="E63" s="364"/>
+      <c r="F63" s="365"/>
+      <c r="G63" s="365"/>
+      <c r="H63" s="366"/>
+      <c r="I63" s="367"/>
+      <c r="J63" s="367"/>
+      <c r="K63" s="368"/>
     </row>
     <row r="64" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="360" t="s">
+      <c r="A64" s="434" t="s">
         <v>380</v>
       </c>
-      <c r="B64" s="361"/>
-      <c r="C64" s="361"/>
+      <c r="B64" s="435"/>
+      <c r="C64" s="435"/>
       <c r="D64" s="125" t="s">
         <v>381</v>
       </c>
@@ -15000,16 +15006,16 @@
       <c r="H64" s="138">
         <v>2</v>
       </c>
-      <c r="I64" s="350" t="s">
+      <c r="I64" s="359" t="s">
         <v>383</v>
       </c>
-      <c r="J64" s="350"/>
-      <c r="K64" s="351"/>
+      <c r="J64" s="359"/>
+      <c r="K64" s="360"/>
     </row>
     <row r="65" spans="1:11" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="362"/>
-      <c r="B65" s="363"/>
-      <c r="C65" s="363"/>
+      <c r="A65" s="436"/>
+      <c r="B65" s="437"/>
+      <c r="C65" s="437"/>
       <c r="D65" s="130" t="s">
         <v>384</v>
       </c>
@@ -15025,18 +15031,18 @@
       <c r="H65" s="139">
         <v>3</v>
       </c>
-      <c r="I65" s="350" t="s">
+      <c r="I65" s="359" t="s">
         <v>386</v>
       </c>
-      <c r="J65" s="350"/>
-      <c r="K65" s="351"/>
+      <c r="J65" s="359"/>
+      <c r="K65" s="360"/>
     </row>
     <row r="66" spans="1:11" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="367" t="s">
+      <c r="A66" s="401" t="s">
         <v>387</v>
       </c>
-      <c r="B66" s="347"/>
-      <c r="C66" s="347"/>
+      <c r="B66" s="402"/>
+      <c r="C66" s="402"/>
       <c r="D66" s="131" t="s">
         <v>388</v>
       </c>
@@ -15052,18 +15058,18 @@
       <c r="H66" s="139" t="s">
         <v>192</v>
       </c>
-      <c r="I66" s="350" t="s">
+      <c r="I66" s="359" t="s">
         <v>390</v>
       </c>
-      <c r="J66" s="350"/>
-      <c r="K66" s="351"/>
+      <c r="J66" s="359"/>
+      <c r="K66" s="360"/>
     </row>
     <row r="67" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="367" t="s">
+      <c r="A67" s="401" t="s">
         <v>391</v>
       </c>
-      <c r="B67" s="347"/>
-      <c r="C67" s="347"/>
+      <c r="B67" s="402"/>
+      <c r="C67" s="402"/>
       <c r="D67" s="91" t="s">
         <v>392</v>
       </c>
@@ -15079,18 +15085,18 @@
       <c r="H67" s="140">
         <v>8</v>
       </c>
-      <c r="I67" s="350" t="s">
+      <c r="I67" s="359" t="s">
         <v>394</v>
       </c>
-      <c r="J67" s="350"/>
-      <c r="K67" s="351"/>
+      <c r="J67" s="359"/>
+      <c r="K67" s="360"/>
     </row>
     <row r="68" spans="1:11" ht="57" x14ac:dyDescent="0.25">
-      <c r="A68" s="385" t="s">
+      <c r="A68" s="407" t="s">
         <v>395</v>
       </c>
-      <c r="B68" s="386"/>
-      <c r="C68" s="387"/>
+      <c r="B68" s="408"/>
+      <c r="C68" s="409"/>
       <c r="D68" s="122" t="s">
         <v>396</v>
       </c>
@@ -15106,37 +15112,37 @@
       <c r="H68" s="139" t="s">
         <v>143</v>
       </c>
-      <c r="I68" s="350" t="s">
+      <c r="I68" s="359" t="s">
         <v>398</v>
       </c>
-      <c r="J68" s="350"/>
-      <c r="K68" s="351"/>
+      <c r="J68" s="359"/>
+      <c r="K68" s="360"/>
     </row>
     <row r="69" spans="1:11" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="347" t="s">
+      <c r="A69" s="402" t="s">
         <v>399</v>
       </c>
-      <c r="B69" s="347"/>
-      <c r="C69" s="347"/>
+      <c r="B69" s="402"/>
+      <c r="C69" s="402"/>
       <c r="D69" s="142" t="s">
         <v>400</v>
       </c>
-      <c r="E69" s="430" t="s">
+      <c r="E69" s="361" t="s">
         <v>401</v>
       </c>
-      <c r="F69" s="431"/>
-      <c r="G69" s="431"/>
-      <c r="H69" s="431"/>
-      <c r="I69" s="431"/>
-      <c r="J69" s="431"/>
-      <c r="K69" s="432"/>
+      <c r="F69" s="362"/>
+      <c r="G69" s="362"/>
+      <c r="H69" s="362"/>
+      <c r="I69" s="362"/>
+      <c r="J69" s="362"/>
+      <c r="K69" s="363"/>
     </row>
     <row r="70" spans="1:11" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="347" t="s">
+      <c r="A70" s="402" t="s">
         <v>402</v>
       </c>
-      <c r="B70" s="347"/>
-      <c r="C70" s="347"/>
+      <c r="B70" s="402"/>
+      <c r="C70" s="402"/>
       <c r="D70" s="121" t="s">
         <v>403</v>
       </c>
@@ -15152,18 +15158,18 @@
       <c r="H70" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="I70" s="350" t="s">
+      <c r="I70" s="359" t="s">
         <v>406</v>
       </c>
-      <c r="J70" s="350"/>
-      <c r="K70" s="350"/>
+      <c r="J70" s="359"/>
+      <c r="K70" s="359"/>
     </row>
     <row r="71" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A71" s="366" t="s">
+      <c r="A71" s="404" t="s">
         <v>407</v>
       </c>
-      <c r="B71" s="366"/>
-      <c r="C71" s="366"/>
+      <c r="B71" s="404"/>
+      <c r="C71" s="404"/>
       <c r="D71" s="122" t="s">
         <v>408</v>
       </c>
@@ -15179,37 +15185,37 @@
       <c r="H71" s="87" t="s">
         <v>410</v>
       </c>
-      <c r="I71" s="350" t="s">
+      <c r="I71" s="359" t="s">
         <v>411</v>
       </c>
-      <c r="J71" s="350"/>
-      <c r="K71" s="350"/>
+      <c r="J71" s="359"/>
+      <c r="K71" s="359"/>
     </row>
     <row r="72" spans="1:11" ht="75.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="347" t="s">
+      <c r="A72" s="402" t="s">
         <v>412</v>
       </c>
-      <c r="B72" s="347"/>
-      <c r="C72" s="347"/>
+      <c r="B72" s="402"/>
+      <c r="C72" s="402"/>
       <c r="D72" s="142" t="s">
         <v>413</v>
       </c>
-      <c r="E72" s="418" t="s">
+      <c r="E72" s="347" t="s">
         <v>401</v>
       </c>
-      <c r="F72" s="419"/>
-      <c r="G72" s="419"/>
-      <c r="H72" s="419"/>
-      <c r="I72" s="419"/>
-      <c r="J72" s="419"/>
-      <c r="K72" s="420"/>
+      <c r="F72" s="348"/>
+      <c r="G72" s="348"/>
+      <c r="H72" s="348"/>
+      <c r="I72" s="348"/>
+      <c r="J72" s="348"/>
+      <c r="K72" s="349"/>
     </row>
     <row r="73" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="347" t="s">
+      <c r="A73" s="402" t="s">
         <v>414</v>
       </c>
-      <c r="B73" s="347"/>
-      <c r="C73" s="347"/>
+      <c r="B73" s="402"/>
+      <c r="C73" s="402"/>
       <c r="D73" s="122" t="s">
         <v>415</v>
       </c>
@@ -15225,37 +15231,37 @@
       <c r="H73" s="87">
         <v>3</v>
       </c>
-      <c r="I73" s="421" t="s">
+      <c r="I73" s="350" t="s">
         <v>417</v>
       </c>
-      <c r="J73" s="422"/>
-      <c r="K73" s="423"/>
+      <c r="J73" s="351"/>
+      <c r="K73" s="352"/>
     </row>
     <row r="74" spans="1:11" ht="300.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="347" t="s">
+      <c r="A74" s="402" t="s">
         <v>418</v>
       </c>
-      <c r="B74" s="347"/>
-      <c r="C74" s="347"/>
+      <c r="B74" s="402"/>
+      <c r="C74" s="402"/>
       <c r="D74" s="121" t="s">
         <v>419</v>
       </c>
-      <c r="E74" s="427" t="s">
+      <c r="E74" s="356" t="s">
         <v>401</v>
       </c>
-      <c r="F74" s="428"/>
-      <c r="G74" s="428"/>
-      <c r="H74" s="428"/>
-      <c r="I74" s="428"/>
-      <c r="J74" s="428"/>
-      <c r="K74" s="429"/>
+      <c r="F74" s="357"/>
+      <c r="G74" s="357"/>
+      <c r="H74" s="357"/>
+      <c r="I74" s="357"/>
+      <c r="J74" s="357"/>
+      <c r="K74" s="358"/>
     </row>
     <row r="75" spans="1:11" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="348" t="s">
+      <c r="A75" s="426" t="s">
         <v>420</v>
       </c>
-      <c r="B75" s="349"/>
-      <c r="C75" s="349"/>
+      <c r="B75" s="427"/>
+      <c r="C75" s="427"/>
       <c r="D75" s="143" t="s">
         <v>421</v>
       </c>
@@ -15271,11 +15277,11 @@
       <c r="H75" s="146">
         <v>7</v>
       </c>
-      <c r="I75" s="424" t="s">
+      <c r="I75" s="353" t="s">
         <v>423</v>
       </c>
-      <c r="J75" s="425"/>
-      <c r="K75" s="426"/>
+      <c r="J75" s="354"/>
+      <c r="K75" s="355"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="89">
@@ -15404,6 +15410,82 @@
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="I60:K60"/>
+    <mergeCell ref="A62:C63"/>
+    <mergeCell ref="A64:C65"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="A52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E37:K37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:K40"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:K38"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:K34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:K35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:K36"/>
+    <mergeCell ref="E31:K31"/>
+    <mergeCell ref="E32:K32"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:K33"/>
+    <mergeCell ref="E25:P25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="D17:P17"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="E18:P18"/>
+    <mergeCell ref="E19:P19"/>
+    <mergeCell ref="E20:P20"/>
+    <mergeCell ref="E21:P21"/>
+    <mergeCell ref="E23:P23"/>
+    <mergeCell ref="E24:P24"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="E15:P15"/>
+    <mergeCell ref="E16:P16"/>
+    <mergeCell ref="E22:P22"/>
     <mergeCell ref="E72:K72"/>
     <mergeCell ref="I73:K73"/>
     <mergeCell ref="I75:K75"/>
@@ -15420,82 +15502,6 @@
     <mergeCell ref="H62:H63"/>
     <mergeCell ref="I62:K63"/>
     <mergeCell ref="I53:K53"/>
-    <mergeCell ref="E25:P25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="D17:P17"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="E18:P18"/>
-    <mergeCell ref="E19:P19"/>
-    <mergeCell ref="E20:P20"/>
-    <mergeCell ref="E21:P21"/>
-    <mergeCell ref="E23:P23"/>
-    <mergeCell ref="E24:P24"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="E15:P15"/>
-    <mergeCell ref="E16:P16"/>
-    <mergeCell ref="E22:P22"/>
-    <mergeCell ref="E31:K31"/>
-    <mergeCell ref="E32:K32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:K33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="E34:K34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:K35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:K36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E37:K37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:K39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="E40:K40"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E38:K38"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I60:K60"/>
-    <mergeCell ref="A62:C63"/>
-    <mergeCell ref="A64:C65"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A66:C66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18945,19 +18951,19 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="445">
+      <c r="A4" s="440">
         <v>0.1</v>
       </c>
       <c r="B4" s="251" t="s">
         <v>1144</v>
       </c>
-      <c r="C4" s="438" t="s">
+      <c r="C4" s="449" t="s">
         <v>1145</v>
       </c>
-      <c r="D4" s="438" t="s">
+      <c r="D4" s="449" t="s">
         <v>1146</v>
       </c>
-      <c r="E4" s="439" t="s">
+      <c r="E4" s="446" t="s">
         <v>1147</v>
       </c>
       <c r="F4" s="272" t="s">
@@ -18974,13 +18980,13 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="445"/>
+      <c r="A5" s="440"/>
       <c r="B5" t="s">
         <v>1151</v>
       </c>
-      <c r="C5" s="438"/>
-      <c r="D5" s="438"/>
-      <c r="E5" s="439"/>
+      <c r="C5" s="449"/>
+      <c r="D5" s="449"/>
+      <c r="E5" s="446"/>
       <c r="F5" t="s">
         <v>1152</v>
       </c>
@@ -18995,48 +19001,48 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="445"/>
+      <c r="A6" s="440"/>
       <c r="B6" t="s">
         <v>1155</v>
       </c>
-      <c r="C6" s="438"/>
-      <c r="D6" s="438"/>
-      <c r="E6" s="439"/>
+      <c r="C6" s="449"/>
+      <c r="D6" s="449"/>
+      <c r="E6" s="446"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="445"/>
+      <c r="A7" s="440"/>
       <c r="B7" t="s">
         <v>1156</v>
       </c>
-      <c r="C7" s="438"/>
-      <c r="D7" s="438"/>
-      <c r="E7" s="439"/>
+      <c r="C7" s="449"/>
+      <c r="D7" s="449"/>
+      <c r="E7" s="446"/>
       <c r="F7" s="272"/>
       <c r="G7" s="188"/>
       <c r="H7" s="271"/>
       <c r="I7" s="188"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="445"/>
+      <c r="A8" s="440"/>
       <c r="B8" s="223" t="s">
         <v>1157</v>
       </c>
-      <c r="C8" s="438"/>
-      <c r="D8" s="438"/>
-      <c r="E8" s="439"/>
+      <c r="C8" s="449"/>
+      <c r="D8" s="449"/>
+      <c r="E8" s="446"/>
       <c r="F8" s="272"/>
       <c r="G8" s="188"/>
       <c r="H8" s="271"/>
       <c r="I8" s="188"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="445"/>
+      <c r="A9" s="440"/>
       <c r="B9" t="s">
         <v>1158</v>
       </c>
-      <c r="C9" s="438"/>
-      <c r="D9" s="438"/>
-      <c r="E9" s="439"/>
+      <c r="C9" s="449"/>
+      <c r="D9" s="449"/>
+      <c r="E9" s="446"/>
       <c r="G9" s="188"/>
       <c r="H9" s="271"/>
       <c r="I9" s="277" t="s">
@@ -19044,13 +19050,13 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="445"/>
+      <c r="A10" s="440"/>
       <c r="B10" s="223" t="s">
         <v>1160</v>
       </c>
-      <c r="C10" s="438"/>
-      <c r="D10" s="438"/>
-      <c r="E10" s="439"/>
+      <c r="C10" s="449"/>
+      <c r="D10" s="449"/>
+      <c r="E10" s="446"/>
       <c r="F10" s="272"/>
       <c r="G10" s="188"/>
       <c r="H10" s="271"/>
@@ -19059,82 +19065,82 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="445"/>
+      <c r="A11" s="440"/>
       <c r="B11" t="s">
         <v>1162</v>
       </c>
-      <c r="C11" s="438"/>
-      <c r="D11" s="438"/>
-      <c r="E11" s="439"/>
+      <c r="C11" s="449"/>
+      <c r="D11" s="449"/>
+      <c r="E11" s="446"/>
       <c r="F11" s="272"/>
       <c r="G11" s="188"/>
       <c r="H11" s="271"/>
       <c r="I11" s="188"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="445"/>
+      <c r="A12" s="440"/>
       <c r="B12" t="s">
         <v>1163</v>
       </c>
-      <c r="C12" s="438"/>
-      <c r="D12" s="438"/>
-      <c r="E12" s="439"/>
+      <c r="C12" s="449"/>
+      <c r="D12" s="449"/>
+      <c r="E12" s="446"/>
       <c r="F12" s="272"/>
       <c r="G12" s="188"/>
       <c r="H12" s="271"/>
       <c r="I12" s="188"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="445"/>
+      <c r="A13" s="440"/>
       <c r="B13" t="s">
         <v>1164</v>
       </c>
-      <c r="C13" s="438"/>
-      <c r="D13" s="438"/>
-      <c r="E13" s="439"/>
+      <c r="C13" s="449"/>
+      <c r="D13" s="449"/>
+      <c r="E13" s="446"/>
       <c r="F13" s="272"/>
       <c r="G13" s="188"/>
       <c r="H13" s="271"/>
       <c r="I13" s="188"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="445"/>
+      <c r="A14" s="440"/>
       <c r="B14" t="s">
         <v>1165</v>
       </c>
-      <c r="C14" s="438"/>
-      <c r="D14" s="438"/>
-      <c r="E14" s="439"/>
+      <c r="C14" s="449"/>
+      <c r="D14" s="449"/>
+      <c r="E14" s="446"/>
       <c r="F14" s="272"/>
       <c r="G14" s="188"/>
       <c r="H14" s="271"/>
       <c r="I14" s="188"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="445"/>
+      <c r="A15" s="440"/>
       <c r="B15" t="s">
         <v>1166</v>
       </c>
-      <c r="C15" s="438"/>
-      <c r="D15" s="438"/>
-      <c r="E15" s="439"/>
+      <c r="C15" s="449"/>
+      <c r="D15" s="449"/>
+      <c r="E15" s="446"/>
       <c r="F15" s="272"/>
       <c r="G15" s="188"/>
       <c r="H15" s="271"/>
       <c r="I15" s="188"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="446">
+      <c r="A16" s="441">
         <v>0.2</v>
       </c>
       <c r="B16" s="252" t="s">
         <v>1167</v>
       </c>
-      <c r="C16" s="438" t="s">
+      <c r="C16" s="449" t="s">
         <v>1168</v>
       </c>
-      <c r="D16" s="439"/>
-      <c r="E16" s="440" t="s">
+      <c r="D16" s="446"/>
+      <c r="E16" s="447" t="s">
         <v>1147</v>
       </c>
       <c r="F16" t="s">
@@ -19145,126 +19151,126 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="446"/>
+      <c r="A17" s="441"/>
       <c r="B17" s="223" t="s">
         <v>1170</v>
       </c>
-      <c r="C17" s="438"/>
-      <c r="D17" s="439"/>
-      <c r="E17" s="440"/>
+      <c r="C17" s="449"/>
+      <c r="D17" s="446"/>
+      <c r="E17" s="447"/>
       <c r="F17" t="s">
         <v>1171</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="446"/>
+      <c r="A18" s="441"/>
       <c r="B18" t="s">
         <v>1172</v>
       </c>
-      <c r="C18" s="438"/>
-      <c r="D18" s="439"/>
-      <c r="E18" s="440"/>
+      <c r="C18" s="449"/>
+      <c r="D18" s="446"/>
+      <c r="E18" s="447"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="446"/>
+      <c r="A19" s="441"/>
       <c r="B19" t="s">
         <v>1173</v>
       </c>
-      <c r="C19" s="438"/>
-      <c r="D19" s="439"/>
-      <c r="E19" s="440"/>
+      <c r="C19" s="449"/>
+      <c r="D19" s="446"/>
+      <c r="E19" s="447"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="446"/>
+      <c r="A20" s="441"/>
       <c r="B20" t="s">
         <v>1174</v>
       </c>
-      <c r="C20" s="438"/>
-      <c r="D20" s="439"/>
-      <c r="E20" s="440"/>
+      <c r="C20" s="449"/>
+      <c r="D20" s="446"/>
+      <c r="E20" s="447"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="446"/>
+      <c r="A21" s="441"/>
       <c r="B21" t="s">
         <v>1175</v>
       </c>
-      <c r="C21" s="438"/>
-      <c r="D21" s="439"/>
-      <c r="E21" s="440"/>
+      <c r="C21" s="449"/>
+      <c r="D21" s="446"/>
+      <c r="E21" s="447"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="446"/>
+      <c r="A22" s="441"/>
       <c r="B22" s="223" t="s">
         <v>1176</v>
       </c>
-      <c r="C22" s="438"/>
-      <c r="D22" s="439"/>
-      <c r="E22" s="440"/>
+      <c r="C22" s="449"/>
+      <c r="D22" s="446"/>
+      <c r="E22" s="447"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="446"/>
+      <c r="A23" s="441"/>
       <c r="B23" s="223" t="s">
         <v>1177</v>
       </c>
-      <c r="C23" s="438"/>
-      <c r="D23" s="439"/>
-      <c r="E23" s="440"/>
+      <c r="C23" s="449"/>
+      <c r="D23" s="446"/>
+      <c r="E23" s="447"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="446"/>
+      <c r="A24" s="441"/>
       <c r="B24" t="s">
         <v>1178</v>
       </c>
-      <c r="C24" s="438"/>
-      <c r="D24" s="439"/>
-      <c r="E24" s="440"/>
+      <c r="C24" s="449"/>
+      <c r="D24" s="446"/>
+      <c r="E24" s="447"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="446"/>
+      <c r="A25" s="441"/>
       <c r="B25" t="s">
         <v>1179</v>
       </c>
-      <c r="C25" s="438"/>
-      <c r="D25" s="439"/>
-      <c r="E25" s="440"/>
+      <c r="C25" s="449"/>
+      <c r="D25" s="446"/>
+      <c r="E25" s="447"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="446"/>
+      <c r="A26" s="441"/>
       <c r="B26" t="s">
         <v>1180</v>
       </c>
-      <c r="C26" s="438"/>
-      <c r="D26" s="439"/>
-      <c r="E26" s="440"/>
+      <c r="C26" s="449"/>
+      <c r="D26" s="446"/>
+      <c r="E26" s="447"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="446"/>
+      <c r="A27" s="441"/>
       <c r="B27" t="s">
         <v>1181</v>
       </c>
-      <c r="C27" s="438"/>
-      <c r="D27" s="439"/>
-      <c r="E27" s="440"/>
+      <c r="C27" s="449"/>
+      <c r="D27" s="446"/>
+      <c r="E27" s="447"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="446"/>
+      <c r="A28" s="441"/>
       <c r="B28" t="s">
         <v>1182</v>
       </c>
-      <c r="C28" s="438"/>
-      <c r="D28" s="439"/>
-      <c r="E28" s="440"/>
+      <c r="C28" s="449"/>
+      <c r="D28" s="446"/>
+      <c r="E28" s="447"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="447">
+      <c r="A29" s="442">
         <v>0.3</v>
       </c>
       <c r="B29" s="256" t="s">
         <v>1183</v>
       </c>
-      <c r="C29" s="441"/>
-      <c r="D29" s="442"/>
-      <c r="E29" s="439" t="s">
+      <c r="C29" s="445"/>
+      <c r="D29" s="448"/>
+      <c r="E29" s="446" t="s">
         <v>1147</v>
       </c>
       <c r="H29" s="274" t="s">
@@ -19272,52 +19278,52 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="447"/>
+      <c r="A30" s="442"/>
       <c r="B30" s="223" t="s">
         <v>1184</v>
       </c>
-      <c r="C30" s="441"/>
-      <c r="D30" s="442"/>
-      <c r="E30" s="439"/>
+      <c r="C30" s="445"/>
+      <c r="D30" s="448"/>
+      <c r="E30" s="446"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="447"/>
+      <c r="A31" s="442"/>
       <c r="B31" t="s">
         <v>1185</v>
       </c>
-      <c r="C31" s="441"/>
-      <c r="D31" s="442"/>
-      <c r="E31" s="439"/>
+      <c r="C31" s="445"/>
+      <c r="D31" s="448"/>
+      <c r="E31" s="446"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="447"/>
+      <c r="A32" s="442"/>
       <c r="B32" s="265" t="s">
         <v>1186</v>
       </c>
-      <c r="C32" s="441"/>
-      <c r="D32" s="442"/>
-      <c r="E32" s="439"/>
+      <c r="C32" s="445"/>
+      <c r="D32" s="448"/>
+      <c r="E32" s="446"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="447"/>
+      <c r="A33" s="442"/>
       <c r="B33" t="s">
         <v>1187</v>
       </c>
-      <c r="C33" s="441"/>
-      <c r="D33" s="442"/>
-      <c r="E33" s="439"/>
+      <c r="C33" s="445"/>
+      <c r="D33" s="448"/>
+      <c r="E33" s="446"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="447"/>
+      <c r="A34" s="442"/>
       <c r="B34" t="s">
         <v>1188</v>
       </c>
-      <c r="C34" s="441"/>
-      <c r="D34" s="442"/>
-      <c r="E34" s="439"/>
+      <c r="C34" s="445"/>
+      <c r="D34" s="448"/>
+      <c r="E34" s="446"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="448">
+      <c r="A35" s="443">
         <v>1.1000000000000001</v>
       </c>
       <c r="B35" s="260" t="s">
@@ -19326,7 +19332,7 @@
       <c r="C35" s="257" t="s">
         <v>1190</v>
       </c>
-      <c r="E35" s="439" t="s">
+      <c r="E35" s="446" t="s">
         <v>1191</v>
       </c>
       <c r="G35" t="s">
@@ -19337,11 +19343,11 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="448"/>
+      <c r="A36" s="443"/>
       <c r="B36" s="223" t="s">
         <v>1193</v>
       </c>
-      <c r="E36" s="439"/>
+      <c r="E36" s="446"/>
       <c r="F36" s="272" t="s">
         <v>1194</v>
       </c>
@@ -19356,11 +19362,11 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="448"/>
+      <c r="A37" s="443"/>
       <c r="B37" t="s">
         <v>1197</v>
       </c>
-      <c r="E37" s="439"/>
+      <c r="E37" s="446"/>
       <c r="F37" s="272" t="s">
         <v>1198</v>
       </c>
@@ -19375,62 +19381,62 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="448"/>
+      <c r="A38" s="443"/>
       <c r="B38" t="s">
         <v>1201</v>
       </c>
-      <c r="E38" s="439"/>
+      <c r="E38" s="446"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="448"/>
+      <c r="A39" s="443"/>
       <c r="B39" t="s">
         <v>1202</v>
       </c>
-      <c r="E39" s="439"/>
+      <c r="E39" s="446"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="448"/>
+      <c r="A40" s="443"/>
       <c r="B40" t="s">
         <v>1203</v>
       </c>
-      <c r="E40" s="439"/>
+      <c r="E40" s="446"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="448"/>
+      <c r="A41" s="443"/>
       <c r="B41" t="s">
         <v>1204</v>
       </c>
-      <c r="E41" s="439"/>
+      <c r="E41" s="446"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="448"/>
+      <c r="A42" s="443"/>
       <c r="B42" t="s">
         <v>1205</v>
       </c>
-      <c r="E42" s="439"/>
+      <c r="E42" s="446"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="448"/>
+      <c r="A43" s="443"/>
       <c r="B43" t="s">
         <v>1206</v>
       </c>
-      <c r="E43" s="439"/>
+      <c r="E43" s="446"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="448"/>
+      <c r="A44" s="443"/>
       <c r="B44" t="s">
         <v>1207</v>
       </c>
-      <c r="E44" s="439"/>
+      <c r="E44" s="446"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="449">
+      <c r="A47" s="444">
         <v>1.2</v>
       </c>
       <c r="B47" s="262" t="s">
         <v>1208</v>
       </c>
-      <c r="E47" s="439" t="s">
+      <c r="E47" s="446" t="s">
         <v>1209</v>
       </c>
       <c r="G47" t="s">
@@ -19441,35 +19447,35 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="449"/>
+      <c r="A48" s="444"/>
       <c r="B48" s="223" t="s">
         <v>1211</v>
       </c>
-      <c r="E48" s="439"/>
+      <c r="E48" s="446"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="449"/>
+      <c r="A49" s="444"/>
       <c r="B49" s="223" t="s">
         <v>1212</v>
       </c>
-      <c r="E49" s="439"/>
+      <c r="E49" s="446"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="449"/>
+      <c r="A50" s="444"/>
       <c r="B50" t="s">
         <v>1213</v>
       </c>
-      <c r="E50" s="439"/>
+      <c r="E50" s="446"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="449"/>
+      <c r="A51" s="444"/>
       <c r="B51" t="s">
         <v>1206</v>
       </c>
-      <c r="E51" s="439"/>
+      <c r="E51" s="446"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="443">
+      <c r="A54" s="438">
         <v>1.3</v>
       </c>
       <c r="B54" s="264" t="s">
@@ -19481,7 +19487,7 @@
       <c r="D54" t="s">
         <v>1216</v>
       </c>
-      <c r="E54" s="440" t="s">
+      <c r="E54" s="447" t="s">
         <v>1217</v>
       </c>
       <c r="G54" t="s">
@@ -19495,41 +19501,41 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="443"/>
+      <c r="A55" s="438"/>
       <c r="B55" s="223" t="s">
         <v>1220</v>
       </c>
-      <c r="E55" s="440"/>
+      <c r="E55" s="447"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="443"/>
+      <c r="A56" s="438"/>
       <c r="B56" t="s">
         <v>1221</v>
       </c>
-      <c r="E56" s="440"/>
+      <c r="E56" s="447"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="443"/>
+      <c r="A57" s="438"/>
       <c r="B57" t="s">
         <v>1222</v>
       </c>
-      <c r="E57" s="440"/>
+      <c r="E57" s="447"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="443"/>
+      <c r="A58" s="438"/>
       <c r="B58" t="s">
         <v>1223</v>
       </c>
-      <c r="E58" s="440"/>
+      <c r="E58" s="447"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="444">
+      <c r="A61" s="439">
         <v>1.4</v>
       </c>
       <c r="B61" s="267" t="s">
         <v>1224</v>
       </c>
-      <c r="E61" s="440" t="s">
+      <c r="E61" s="447" t="s">
         <v>1225</v>
       </c>
       <c r="G61" t="s">
@@ -19540,38 +19546,38 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="444"/>
+      <c r="A62" s="439"/>
       <c r="B62" s="223" t="s">
         <v>1227</v>
       </c>
-      <c r="E62" s="440"/>
+      <c r="E62" s="447"/>
       <c r="G62" s="257" t="s">
         <v>1228</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="444"/>
+      <c r="A63" s="439"/>
       <c r="B63" t="s">
         <v>1229</v>
       </c>
-      <c r="E63" s="440"/>
+      <c r="E63" s="447"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="444"/>
+      <c r="A64" s="439"/>
       <c r="B64" t="s">
         <v>1230</v>
       </c>
-      <c r="E64" s="440"/>
+      <c r="E64" s="447"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="444"/>
+      <c r="A65" s="439"/>
       <c r="B65" t="s">
         <v>1231</v>
       </c>
-      <c r="E65" s="440"/>
+      <c r="E65" s="447"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="445">
+      <c r="A67" s="440">
         <v>1.5</v>
       </c>
       <c r="B67" s="251" t="s">
@@ -19582,19 +19588,19 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="445"/>
+      <c r="A68" s="440"/>
       <c r="B68" s="223" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="445"/>
+      <c r="A69" s="440"/>
       <c r="B69" t="s">
         <v>1234</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="446">
+      <c r="A72" s="441">
         <v>1.6</v>
       </c>
       <c r="B72" s="252" t="s">
@@ -19611,7 +19617,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="446"/>
+      <c r="A73" s="441"/>
       <c r="B73" s="223" t="s">
         <v>1238</v>
       </c>
@@ -19626,7 +19632,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="446"/>
+      <c r="A74" s="441"/>
       <c r="B74" t="s">
         <v>1240</v>
       </c>
@@ -19644,13 +19650,13 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="446"/>
+      <c r="A75" s="441"/>
       <c r="B75" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="446"/>
+      <c r="A76" s="441"/>
       <c r="B76" t="s">
         <v>1244</v>
       </c>
@@ -20019,6 +20025,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="D4:D15"/>
+    <mergeCell ref="E4:E15"/>
+    <mergeCell ref="C16:C28"/>
+    <mergeCell ref="E16:E28"/>
+    <mergeCell ref="D16:D28"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="E35:E44"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="E54:E58"/>
+    <mergeCell ref="E61:E65"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="A61:A65"/>
     <mergeCell ref="A67:A69"/>
@@ -20028,19 +20047,6 @@
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A44"/>
     <mergeCell ref="A47:A51"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="E35:E44"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="E54:E58"/>
-    <mergeCell ref="E61:E65"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="C4:C15"/>
-    <mergeCell ref="D4:D15"/>
-    <mergeCell ref="E4:E15"/>
-    <mergeCell ref="C16:C28"/>
-    <mergeCell ref="E16:E28"/>
-    <mergeCell ref="D16:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20173,11 +20179,11 @@
   <sheetPr>
     <tabColor rgb="FFFF9999"/>
   </sheetPr>
-  <dimension ref="A1:BU8"/>
+  <dimension ref="A1:BV8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20186,23 +20192,23 @@
     <col min="2" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="230" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="230" customWidth="1"/>
-    <col min="9" max="9" width="47" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="230" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.85546875" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" customWidth="1"/>
-    <col min="14" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="50.42578125" customWidth="1"/>
-    <col min="20" max="20" width="80.85546875" customWidth="1"/>
+    <col min="6" max="7" width="45.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="230" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="230" customWidth="1"/>
+    <col min="10" max="10" width="47" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="230" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="15" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="50.42578125" customWidth="1"/>
+    <col min="21" max="21" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="4" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:74" s="4" customFormat="1" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="288" t="s">
         <v>101</v>
       </c>
@@ -20221,49 +20227,51 @@
       <c r="F1" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="284" t="s">
+      <c r="G1" s="283" t="s">
+        <v>1306</v>
+      </c>
+      <c r="H1" s="284" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="284" t="s">
+      <c r="I1" s="284" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="283" t="s">
+      <c r="J1" s="283" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="284" t="s">
+      <c r="K1" s="284" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="283" t="s">
+      <c r="L1" s="283" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="283" t="s">
+      <c r="M1" s="283" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="285" t="s">
+      <c r="N1" s="285" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="281" t="s">
+      <c r="O1" s="281" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="R1" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="S1" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1"/>
       <c r="V1"/>
       <c r="W1"/>
       <c r="X1"/>
@@ -20316,8 +20324,9 @@
       <c r="BS1"/>
       <c r="BT1"/>
       <c r="BU1"/>
-    </row>
-    <row r="2" spans="1:73" s="4" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BV1"/>
+    </row>
+    <row r="2" spans="1:74" s="4" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>120</v>
       </c>
@@ -20336,31 +20345,29 @@
       <c r="F2" s="290" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="450"/>
+      <c r="H2" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="L2" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="76" t="s">
-        <v>121</v>
-      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
       <c r="O2" s="76" t="s">
         <v>121</v>
       </c>
       <c r="P2" s="76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q2" s="76" t="s">
         <v>123</v>
@@ -20368,11 +20375,13 @@
       <c r="R2" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="167" t="s">
+      <c r="S2" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="T2" s="167" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="89"/>
-      <c r="U2"/>
+      <c r="U2" s="89"/>
       <c r="V2"/>
       <c r="W2"/>
       <c r="X2"/>
@@ -20425,8 +20434,9 @@
       <c r="BS2"/>
       <c r="BT2"/>
       <c r="BU2"/>
-    </row>
-    <row r="3" spans="1:73" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="BV2"/>
+    </row>
+    <row r="3" spans="1:74" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>125</v>
       </c>
@@ -20445,31 +20455,29 @@
       <c r="F3" s="287" t="s">
         <v>1304</v>
       </c>
-      <c r="G3" s="294" t="s">
+      <c r="G3" s="287"/>
+      <c r="H3" s="294" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="294" t="s">
+      <c r="I3" s="294" t="s">
         <v>127</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="J3" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="J3" s="98" t="s">
+      <c r="K3" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="18" t="s">
+      <c r="L3" s="37"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="N3" s="76" t="s">
+      <c r="O3" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="O3" s="76" t="s">
+      <c r="P3" s="76" t="s">
         <v>121</v>
-      </c>
-      <c r="P3" s="76" t="s">
-        <v>123</v>
       </c>
       <c r="Q3" s="76" t="s">
         <v>123</v>
@@ -20477,10 +20485,12 @@
       <c r="R3" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="S3" s="167" t="s">
+      <c r="S3" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="T3" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="U3"/>
       <c r="V3"/>
       <c r="W3"/>
       <c r="X3"/>
@@ -20513,7 +20523,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
       <c r="BA3"/>
-      <c r="BC3"/>
+      <c r="BB3"/>
       <c r="BD3"/>
       <c r="BE3"/>
       <c r="BF3"/>
@@ -20532,51 +20542,52 @@
       <c r="BS3"/>
       <c r="BT3"/>
       <c r="BU3"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="T4" s="110"/>
-    </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="T5" s="110"/>
-    </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="T6" s="110"/>
-    </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="T7" s="110"/>
-    </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="T8" s="110"/>
+      <c r="BV3"/>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="U4" s="110"/>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="U5" s="110"/>
+    </row>
+    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="U6" s="110"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="U7" s="110"/>
+    </row>
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="U8" s="110"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R3" xr:uid="{9C7276AA-1D31-45CB-99BE-1EB8F29BD1DF}"/>
-  <conditionalFormatting sqref="N4:P8">
+  <autoFilter ref="A1:S3" xr:uid="{9C7276AA-1D31-45CB-99BE-1EB8F29BD1DF}"/>
+  <conditionalFormatting sqref="O4:Q8">
     <cfRule type="containsText" dxfId="45" priority="30" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",N4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("No",O4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:S3">
+  <conditionalFormatting sqref="O2:T3">
     <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",N2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("No",O2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="43" priority="25" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",N2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",O2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="42" priority="26" operator="containsText" text="n/a">
-      <formula>NOT(ISERROR(SEARCH("n/a",N2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("n/a",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{AFCBC948-B92C-DA44-ABCA-2FBB2AF0F67A}">
       <formula1>Modules</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{116FBC48-4136-4D46-ACB6-C7DCCA330309}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3" xr:uid="{116FBC48-4136-4D46-ACB6-C7DCCA330309}">
       <formula1>Conformance</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{6286BF4D-0400-4248-A507-BD9F076D18EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{6286BF4D-0400-4248-A507-BD9F076D18EB}">
       <formula1>QuestionType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{C0758AB3-0611-5D47-86A7-F99474B743C6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{C0758AB3-0611-5D47-86A7-F99474B743C6}">
       <formula1>DataType</formula1>
     </dataValidation>
   </dataValidations>
@@ -20590,13 +20601,13 @@
           <x14:formula1>
             <xm:f>lists!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>J9:J130</xm:sqref>
+          <xm:sqref>K9:K130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49E6843B-091C-F84C-B7A4-6E06EA5FD96A}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G49</xm:sqref>
+          <xm:sqref>H9:H49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -23766,6 +23777,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F9864B29171A641B582E76D46C7ACA2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40ac230278d261affbe351c37d5a0641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3fd76951-e4f7-4cc9-8ccb-c4998aa78893" xmlns:ns3="3092193c-6f29-485f-87d2-f467a52e3379" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a5fd78be80f9e1db3d79d02d2c3a784" ns2:_="" ns3:_="">
     <xsd:import namespace="3fd76951-e4f7-4cc9-8ccb-c4998aa78893"/>
@@ -23942,15 +23962,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB274D9-D29B-4016-B1A7-8FC633794465}">
   <ds:schemaRefs>
@@ -23969,6 +23980,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21961765-F20D-4C30-82DC-BD9CF7E6DDAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21444850-BD52-4C83-86F6-A4900F7D7F4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23985,12 +24004,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21961765-F20D-4C30-82DC-BD9CF7E6DDAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>